<commit_message>
Update to latest flashcards
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - KS Oeffentliches Recht I (JKU, Austria).xlsx
+++ b/flashcards/Memcode - KS Oeffentliches Recht I (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="500">
   <si>
     <t>Question</t>
   </si>
@@ -19,6 +19,192 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Selbständige Verordnung&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ergehen unmittelbar aus Bundesverfassung (ohne weitere Gesetze)&lt;/li&gt;&lt;li&gt;Gesetzesergänzend, gesetzesvertretend oder gesetzesändernd.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Rechtsverordnung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Wirkt nach außen&lt;/li&gt;&lt;li&gt;Legt Rechte und Pflichten für Bürger fest&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Ortspolizeiliche Verordnung&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Von Gemeinden erlassen &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(Art. 118 Abs. 6)&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;im eigenen Wirkungsbereich&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;nur zur Abwehr drohender oder bestehender Missstände&lt;/li&gt;&lt;li class="ql-indent-1"&gt;dürfen nicht gegen Bundes- oder Landesrecht verstoßen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Arten von Verordnungen&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Durchführungsverordnung &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Selbständige Verordnung&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Ortspolizeiliche Verordnung&lt;/li&gt;&lt;li&gt;Rechtsverordnung&lt;/li&gt;&lt;li&gt;Verwaltungsverordnung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Landesverwaltung: Landesregierung (Zuständigkeit, Zusammensetzung, Entscheidungsfindung, Wahl, Regierungsart, Amt)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Oberstes Organ der Landesverwaltung, zuständig für hoheitliche (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel11" rel="noopener noreferrer" target="_blank"&gt;Art. 11-15 B-VG&lt;/a&gt;) und nicht hoheitliche (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel17" rel="noopener noreferrer" target="_blank"&gt;Art. 17 B-VG&lt;/a&gt;) Verwaltung&lt;/li&gt;&lt;li&gt;Besteht aus Landeshauptmann und weiteren Landesräten (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel101" rel="noopener noreferrer" target="_blank"&gt;Art. 101 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Entscheidet als Kollegialorgan, Landesräte können teilweise auch als Einzelorgane tätig werden (Ämter der Landesregierungen)&lt;/li&gt;&lt;li&gt;Parlamentarisches System: Landtag wählt Regierung &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel101" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;Art. 101 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Meist Mehrheitsregierung, außer in OÖ, NÖ und W → Proporzregierung=Konzentrationsregierung&lt;/li&gt;&lt;li&gt;Amt der Landesregierung: Hilfsapparat der Regierung &lt;strong&gt;&lt;em&gt;und &lt;/em&gt;&lt;/strong&gt;des Landeshauptmanns.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Grundrechtsquellen: Grundrechte im B-VG&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gleichheitssatz (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel7" rel="noopener noreferrer" target="_blank"&gt;Art. 7 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Recht auf den gesetzlichen Richter (&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel83" rel="noopener noreferrer" target="_blank" style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Art. 83 Abs. 2 B-VG&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Recht der Richter auf Unabhängigkeit (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel87" rel="noopener noreferrer" target="_blank"&gt;Art. 87 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Recht der Gemeinden auf Selbstverwaltung (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank"&gt;Art. 116 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Weisungsfreie Vollziehung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Unabhängige &lt;strong&gt;Richter &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel87" rel="noopener noreferrer" target="_blank"&gt;Art. 87 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;weisungsfreier Teil der &lt;strong&gt;Justizverwaltung &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel87" rel="noopener noreferrer" target="_blank"&gt;Art. 87 Abs. 2 B-VG&lt;/a&gt;): Richtersenate und Kommissionen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gemeindeselbstverwaltung&lt;/strong&gt;: Gemeinderat und Bürgermeister (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;Art. 116 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Weisungsfrei, unterliegen nur Aufsicht der Bundes/Landesbehörden.&lt;/li&gt;&lt;li&gt;Einfacher Bundes/Landesgesetzgeber kann weitere Verwaltungsorgane bei Rechtfertigung weisungsfrei stellen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel20" rel="noopener noreferrer" target="_blank"&gt;Art. 20 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie regelt die (Finanz)Verfassung wie der Staat zu seinem Geld kommt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Konstruiert den Staat als Abgabestaat&lt;/li&gt;&lt;li&gt;Staat bringt das Geld zwangsweise durch hoheitliche Abgaben, Gebühren und Beiträge auf.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie wird das Budget bestimmt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In einem Budgetgesetz (Bundesfinanzgesetz) auf der Grundlage eines Bundesfinanzrahmengesetzes&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie nennt man das Geld- und Vermögensrelevante Handeln der Verwaltung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gebarung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wo liegt die Budgethoheit, was bedeutet sie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Beim Parlament, das Parlament entscheidet, wofür die Verwaltung welche Summen ausgeben darf. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sind Gemeinden unter dem Grundrechtsschutz?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ja, die Gemeindeautonomie (Recht auf Selbstverwaltung, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank"&gt;Art. 116 Abs. 1 B-VG&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer ist ausgenommen aus dem Grundrechtsschutz?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Staaten (Bund und Land), die Grundrechte sind nicht dazu da den Staat vor sich selbst, Land vor dem Bund oder Bund vor dem Land zu schützen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Können Gebietskörperschaften Träger von Grundrechten sein?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ja, juristische Personen&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (des öffentlichen und des Privatrechts)&lt;/span&gt; können Träger von Grundrechten sein, wenn dies &lt;strong&gt;wesensmäßig &lt;/strong&gt;möglich ist.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gilt der Gleichheitssatz auch für die nicht-hoheitliche Verwaltung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ja, Diskriminierung ist verboten, und Sachlichkeit wird verlangt. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Fiskalgeltung der Grundrechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Bindung des Staates an die Grundrechte im Rahmen der Privatwirtschaftsverwaltung.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Verwaltung kann sowohl hoheitlich als auch privatrechtlich Handeln. Gilt der Grundrechtsschutz auch gegen die nicht-hoheitlichen Handlungen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ja&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie nennt man Verwaltungsakte des BP?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Entschließungen&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Verwaltungsapparat des BP?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Präsidentschaftskanzl&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;ei&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine formalgesetzliche Delegation?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ein Gesetz bestimmt das Handeln der Vollziehung nicht oder nur sehr ungenau, dies ist verfassungswidrig (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel18" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(105, 122, 180);"&gt;Art 18. Abs 1. B-VG&lt;/a&gt;). Der Gesetzgeber delegiert daher die Pflicht das Recht zu bestimmen an die Vollziehung.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Organisation&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Abstrakte Konstrukte der Rechtsordnung denen bestimmte Aufgaben zukommen, bestehen meist aus vielen Organen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;z.B.: Gebietskörperschaft, Verwaltungsorganisation, Gerichtsorganisation&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sicherheitsverwaltung: Was is das Bundesheer? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;militärische Formation des Bundes, zählt zur unmittelbaren Bundesverwaltung&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sicherheitsbehörden des Bundes&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78a" rel="noopener noreferrer" target="_blank"&gt;Art. 78a-c B-VG&lt;/a&gt; richten die Sicherheitsbehörden ein&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/spg/paragraf/2" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;2 Abs. 2 SPG&lt;/a&gt; definiert Aufgaben der Sicherheitsverwaltung&lt;/li&gt;&lt;li&gt;2/3 Ebenen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;BM für Inneres&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Landespolizeidirektion&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bezirksverwaltungsbehörde&lt;/li&gt;&lt;li&gt;Mischform aus mittelbarer und unmittelbarer Bundesverwaltung, weil auf unterer Ebene teilweise Bezirksverwaltungsbehörden als Landesbehörden eingebunden sind&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Organwalter (Definition, Zuordnung, Arten)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Den abstrakten Organen werden konkrete Menschen zugeordnet. &lt;/li&gt;&lt;li&gt;Gesetzessprache verwendet Organ und Organwalter oft synonym&lt;/li&gt;&lt;li&gt;Immer einer Gebietskörperschaft zugeordnet&lt;/li&gt;&lt;li&gt;Arten (Gesamtbegriff &lt;strong&gt;öffentliche Bedienstete&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Beamte = ernannte berufsmäßige Organe&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vertragsbedienstete = vertraglich bestellte Organe&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;Durchführungsverordnung &lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Präzisiert ein Gesetz (&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel18" rel="noopener noreferrer" target="_blank" style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Art. 18 Abs. 2 B-VG&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;)&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kompetenzverteilung in der nicht-hoheitlichen Verwaltung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel17" rel="noopener noreferrer" target="_blank"&gt;Art. 17 B-VG&lt;/a&gt;: Kompetenzverteilung in Art. 10 - 15 B-VG gilt &lt;strong&gt;nicht&lt;/strong&gt; für nicht-hoheitliche Verwaltung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das hoheitliche Organisationsrecht einer Gebietskörperschaft?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Bestimmt die innere Willensbildung des &lt;strong&gt;privatrechtlichen&lt;/strong&gt; Handelns&lt;/li&gt;&lt;li&gt;Zuständigkeit für Kaufverträge, Willensbildung, inhaltliche Gestaltung von Verträgen ⇾ bestimmt das hoheitliche Organisationsrecht (nicht die Privatrechtsordnung)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktioniert das Gesetzmäßigkeitsgebot in der nicht-hoheitlichen Verwaltung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Geregelt durch das Verwaltungsprivatrecht&lt;/li&gt;&lt;li&gt;&lt;strong&gt;differenziertes Legalitätsprinzip: &lt;/strong&gt;Auch privatrechtliche Handlungen unterliegen dem Gesetzmäßigkeitsgebot,  es ist aber flexibler und weniger streng, als für hoheitliches Handeln &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Inhalt der nicht-hoheitlichen Verwaltung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Privatwirtschaftsverwaltung&lt;/li&gt;&lt;li&gt;Fiskalverwaltung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer kann nicht-hoheitlich handeln, wer nicht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Nur die juristischen Personen: Bund, Länder und Gemeinden, also nur die Verwaltung. &lt;/li&gt;&lt;li&gt;Parlamente und Gerichte handeln  immer hoheitlich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Gebietskörperschaften sind Träger von Privatrechten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel17" rel="noopener noreferrer" target="_blank"&gt;Art. 17 B-VG&lt;/a&gt;: Bund und Länder sind juristische Personen&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank"&gt;Art. 116 Abs. 2 B-VG&lt;/a&gt;: Gemeinden sind juristische Personen&lt;/li&gt;&lt;li&gt;Vermögensfähig sind also der Bund, die Länder und die Gemeinden, nicht der Gesamtstaat Österreich.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was sind die Unterschiede zwischen juristischen Personen des Privatrechts und des öffentlichen Rechts? Was ist identisch? &lt;/p&gt;</t>
   </si>
   <si>
@@ -43,7 +229,7 @@
     <t>&lt;p&gt;Die Privatrechtsordnung erlaubt, dass juristische Personen von der Rechtsordnung als Rechtsträger behandelt wären, als wären sie Menschen.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was sind juristische Personen? Wie wird entschieden, welche juristischen Personen es gibt? &lt;/p&gt;</t>
+    <t>&lt;p&gt;Was sind juristische Personen? &lt;/p&gt;&lt;p&gt;Wie werden sie noch genannt?&lt;/p&gt;&lt;p&gt;Wie wird entschieden, welche juristischen Personen es gibt?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;= virtuelle Menschen&lt;/li&gt;&lt;li&gt;Auch Rechtsperson oder Körperschaft genannt&lt;/li&gt;&lt;li&gt;Gesetzgebung entscheidet ob und welche juristischen Personen es gibt.&lt;/li&gt;&lt;/ul&gt;</t>
@@ -64,13 +250,13 @@
     <t>&lt;p&gt;Wer ist der gesetzliche Vertreter für ein Kind?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Die Eltern (§ 167 ABGB)&lt;/p&gt;</t>
+    <t>&lt;p&gt;Die Eltern (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/167" rel="noopener noreferrer" target="_blank"&gt;§ 167 ABGB&lt;/a&gt;)&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Ist jeder Mensch handlungsfähig?&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Nein (§&amp;nbsp;21 ABGB), wer nicht handlungsfähig ist, braucht einen Vertreter der für ihn handelt&lt;/p&gt;</t>
+    <t>&lt;p&gt;Nein (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/21" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;21 ABGB&lt;/a&gt;), wer nicht handlungsfähig ist, braucht einen Vertreter der für ihn handelt&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist die Handlungsfähigkeit?&lt;/p&gt;</t>
@@ -79,10 +265,10 @@
     <t>&lt;ul&gt;&lt;li&gt;Die Fähigkeit, durch eigenes Handeln Rechte zu erwerben und Pflichten zu begründen.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die Rechtsfähigkeit? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die Fähigkeit, Träger privater Rechte und Pflichten zu sei (z.B.: Eigentümer von Geld und Vermögen)&lt;/li&gt;&lt;li&gt;Jeder Mensch ist von Geburt bis zum Tod rechtsfähig.&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;Was ist die Rechtsfähigkeit? Wer hat sie wie lange? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die Fähigkeit, Träger privater Rechte und Pflichten zu sein (z.B.: Eigentümer von Geld und Vermögen)&lt;/li&gt;&lt;li&gt;Jeder Mensch ist von Geburt bis zum Tod rechtsfähig.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Einzelne Grundrechte&lt;/p&gt;</t>
@@ -91,12 +277,6 @@
     <t>&lt;ul&gt;&lt;li&gt;Eigentumsfreiheit&lt;/li&gt;&lt;li&gt;Erwerbsfreiheit&lt;/li&gt;&lt;li&gt;Recht auf persönliche Freiheit&lt;/li&gt;&lt;li&gt;Hausrecht&lt;/li&gt;&lt;li&gt;Versammlungsfreiheit&lt;/li&gt;&lt;li&gt;Meinungsfreiheit&lt;/li&gt;&lt;li&gt;...&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Grundrechtsquellen: Grundrechte im B-VG&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Gleichheitssatz&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Recht auf den gesetzlichen Richter&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Recht der Richter auf Unabhängigkeit&lt;/li&gt;&lt;li&gt;Recht der Gemeinden auf Selbstverwaltung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist das &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Recht auf den gesetzlichen Richter?&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
@@ -145,6 +325,12 @@
     <t>&lt;p&gt;Präsenz 1/2, Konsens 2/3 (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel99" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 99 Abs. 2 B-VG&lt;/a&gt;)&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
   </si>
   <si>
+    <t>&lt;p&gt;Zuständigkeit&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die &lt;strong&gt;Möglichkeit&lt;/strong&gt; einer Organisation in einer Sache zu handeln&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was sind die Arten der Leitung der Verwaltung?&lt;/p&gt;</t>
   </si>
   <si>
@@ -157,6 +343,48 @@
     <t>&lt;ul&gt;&lt;li&gt;Verfassungsbegriff (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel130" rel="noopener noreferrer" target="_blank"&gt;Art. 130 Abs. 1 B-VG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel132" rel="noopener noreferrer" target="_blank"&gt;Art. 132 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;3 formale Merkmale (nicht vorhanden: Absolut nichtig)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es muss eine Verwaltungsbehörde handeln&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es muss an einen individuellen Adressaten gerichtet sein&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es muss eine behördliche Anordnung enthalten&lt;/li&gt;&lt;li&gt;Gesetzgeber kann weitere Merkmale hinzufügen, Auswirkung des Fehlens legt Gesetzgeber fest (z.B.: relativ nichtig)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
+    <t>&lt;p&gt;Aufgabe&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Organisation &lt;strong&gt;soll&lt;/strong&gt; in einer Sache handeln&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Pflichtaufgabe: muss Handeln&lt;/li&gt;&lt;li class="ql-indent-1"&gt;öffentliche Aufgabe: im Interesse der Allgemeinheit&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Staatliche Aufgabe&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Öffentliche Aufgabe, die der Gesetzgeber dem Staat zuweist&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Verwaltungsaufgabe&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Staatliche Aufgabe der Verwaltung einer Gebietskörperschaft&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Behörde&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Verwaltungsorgane mit Rechtssetzungsbefugnissen (handeln hoheitlich)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Amt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Einer Behörde zugeordneter bürokratischer Hilfsapparat, handelt nicht selbst hoheitlich. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Approbationsbefugnis&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Innerbehördliches Mandat&lt;/li&gt;&lt;li&gt;Organwalter kann Aufgaben an das Amt übertragen&lt;/li&gt;&lt;li&gt;Approbationsbefugte Beamte können damit "im Auftrag" der Behörde Bescheide oder Verordnungen erlassen, der Organwalter ist jedoch immer weisungsbefugt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Formen des Verwaltungshandelns&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Bescheid&lt;/li&gt;&lt;li&gt;Verordnung&lt;/li&gt;&lt;li&gt;Maßnahme&lt;/li&gt;&lt;li&gt;Schlicht-hoheitliches Handeln&lt;/li&gt;&lt;li&gt;(Verwaltungsrechtlicher Vertrag)&lt;/li&gt;&lt;li&gt;Privatrechtliches Handeln&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Eingriffsvorbehalt vs. Ausgestaltungsvorbehalt bei Freiheitsrechten&lt;/p&gt;</t>
   </si>
   <si>
@@ -349,6 +577,18 @@
     <t>&lt;p&gt;&lt;strong&gt;1789&lt;/strong&gt;: Deklaration der Menschen- und Bürgerrechte&lt;/p&gt;&lt;p&gt;&lt;strong&gt;1867&lt;/strong&gt;: Staatsgrundgesetz (Dezemberverfassung) &lt;/p&gt;&lt;p&gt;&lt;strong&gt;1948&lt;/strong&gt;: Allgemeine Erklärung der Menschenrechte&lt;/p&gt;&lt;p&gt;&lt;strong&gt;1950&lt;/strong&gt;: Europäische Menschenrechtskonvention&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
   </si>
   <si>
+    <t>&lt;p&gt;Arten von Bescheiden&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Leistungsbescheid&lt;/strong&gt;: ordnet Tun oder Unterlassen an, &lt;strong&gt;vollstreckbar&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gestaltungsbescheid&lt;/strong&gt;: Gestaltet eine Rechtslage neu, &lt;strong&gt;nicht vollstreckbar&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Feststellungsbescheid&lt;/strong&gt;: verbindliche Feststellung einer unklaren Rechtslage, &lt;strong&gt;nicht vollstreckbar&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Verwaltungshandeln: Verordnung&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Verfassungsbegriff (Art. 139 B-VG)&lt;/li&gt;&lt;li&gt;Generelle (abstrakte oder konkrete) Anordnung einer Verwaltungsbehörde&lt;/li&gt;&lt;li&gt;Erst mit Kundmachung gültig&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;&lt;span style="background-color: rgb(34, 38, 74); color: rgb(238, 236, 246);"&gt;Wachkörper: &lt;/span&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Gemeindewachkörper &lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
@@ -373,12 +613,6 @@
     <t>&lt;ul&gt;&lt;li&gt;Bewaffnete Formationen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78d" rel="noopener noreferrer" target="_blank"&gt;Art. 78d Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bundespolizei: &lt;strong&gt;Bund&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Justizwache: &lt;strong&gt;Bund&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gemeindewachkörper: &lt;strong&gt;Gemeinde&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Organisation und Führung der Bundespolizei und die Org. sonstiger Wachkörper (Ausnahme: Gemeindewachkörper) ist Bundessache&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Sicherheitsbehörden des Bundes&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78a" rel="noopener noreferrer" target="_blank"&gt;Art. 78a-c B-VG&lt;/a&gt; richten die Sicherheitsbehörden ein&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/spg/paragraf/2" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;2 Abs. 2 SPG&lt;/a&gt; definiert Aufgaben der Sicherheitsverwaltung&lt;/li&gt;&lt;li&gt;2/3 Ebenen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;BM für Inneres&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Landespolizeidirektion &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bezirksverwaltungsbehörde&lt;/li&gt;&lt;li&gt;Mischform aus mittelbarer und unmittelbarer Bundesverwaltung, weil auf unterer Ebene teilweise Bezirksverwaltungsbehörden als Landesbehörden eingebunden sind&lt;/li&gt;&lt;li&gt;Bundesheer: militärische Formation des Bundes, zählt zur unmittelbaren Bundesverwaltung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Sicherheitsbehörden: &lt;/span&gt;Bezirksverwaltungsbehörde&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
   </si>
   <si>
@@ -457,12 +691,6 @@
     <t>&lt;ul&gt;&lt;li&gt;Landesverwaltung in Verwaltungssprengel territorial gegliedert&lt;/li&gt;&lt;li&gt;Land in Bezirke gegliedert, 2 Arten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bezirk&lt;/strong&gt;, der mehrere Gemeinden erfasst&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Statutarstadt&lt;/strong&gt;, die alleine ein Bezirk ist&lt;/li&gt;&lt;li&gt;Bezirksverwaltungsbehörden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bezirkshauptmann (monokratisch), Amt: Bezirkshauptmannschaft&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bürgermeister, Amt: Magistrat&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Landesverwaltung: Landesregierung (Zuständigkeit, Zusammensetzung, Entscheidungsfindung, Wahl, Regierungsart, Amt)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Oberstes Organ der Landesverwaltung, zuständig für hoheitliche (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel11" rel="noopener noreferrer" target="_blank"&gt;Art. 11-15 B-VG&lt;/a&gt;) und nicht hoheitliche (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel17" rel="noopener noreferrer" target="_blank"&gt;Art. 17 B-VG&lt;/a&gt;) Verwaltung&lt;/li&gt;&lt;li&gt;Besteht aus Landeshauptmann und weiteren Landesräten  (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel101" rel="noopener noreferrer" target="_blank"&gt;Art. 101 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Entscheidet als Kollegialorgan, Landesräte können teilweise auch als Einzelorgane tätig werden (Ämter der Landesregierungen)&lt;/li&gt;&lt;li&gt;Parlamentarisches System: Landtag wählt Regierung&lt;/li&gt;&lt;li&gt;Meist Mehrheitsregierung, außer in OÖ, NÖ und W → Proporzregierung=Konzentrationsregierung&lt;/li&gt;&lt;li&gt;Amt der Landesregierung: Hilfsapparat der Regierung &lt;strong&gt;&lt;em&gt;und &lt;/em&gt;&lt;/strong&gt;des Landeshauptmanns.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Sicherheitsverwaltung&lt;/p&gt;</t>
   </si>
   <si>
@@ -505,12 +733,6 @@
     <t>&lt;ul&gt;&lt;li&gt;Allzuständigkeit der Staatsgewalt, erledigt von allgemeinen staatlichen Verwaltungsorganen&lt;/li&gt;&lt;li&gt;der Länder: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bezirksverwaltungsbehörden (1. Instanz) &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Landesregierungen (2. Instanz)&lt;/li&gt;&lt;li&gt;der Bund:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bezirksverwaltungsbehörden (1. Instanz)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Landeshauptmann (2. Instanz)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bundesminister (3. Instanz) &lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Weisungsfreie Vollziehung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Unabhängige &lt;strong&gt;Richter &lt;/strong&gt;(Art. 87 Abs. 1 B-VG)&lt;/li&gt;&lt;li&gt;weisungsfreier Teil der &lt;strong&gt;Justizverwaltung &lt;/strong&gt;(Art. 87 Abs. 2 B-VG): Richtersenate und Kommissionen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gemeindeselbstverwaltung&lt;/strong&gt;: Gemeinderat und Bürgermeister.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Weisungsfrei, unterliegen nur Aufsicht der Bundes/Landesbehörden.&lt;/li&gt;&lt;li&gt;Einfacher Bundes/Landesgesetzgeber kann weitere Verwaltungsorgane bei Rechtfertigung weisungsfrei stellen (Art. 20 Abs. 2 B-VG)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Organ&lt;/p&gt;</t>
   </si>
   <si>
@@ -541,108 +763,6 @@
     <t>&lt;ul&gt;&lt;li&gt;Wirkt nach innen, regelt die interne Verwaltungsorganisation&lt;/li&gt;&lt;li&gt;muss nicht kundgemacht werden (Abgrenzung zur Weisung schweirig)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Rechtsverordnung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Wirkt nach außen&lt;/li&gt;&lt;li&gt;Legt Rechte und Pflichten für Bürger fest&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Ortspolizeiliche Verordnung&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Von Gemeinden erlassen &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(Art. 118 Abs. 6)&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;im eigenen Wirkungsbereich&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;nur zur Abwehr drohender oder bestehender Missstände&lt;/li&gt;&lt;li class="ql-indent-1"&gt;dürfen nicht gegen Bundes- oder Landesrecht verstoßen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Selbständige Verordnung&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Ergehen unmittelbar aus Bundesverfassung (ohne weitere Gesetze)&lt;/li&gt;&lt;li&gt;Gesetzesergänzend, gesetzesvertretend oder gesetzesändernd.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;Durchführungsverordnung &lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Präzisiert ein Gesetz (Art. 18 Abs. 2 B-VG)&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Arten von Verordnungen&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Durchführungsverordnung &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Selbständige Verordnung&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Ortspolizeiliche Verordnung&lt;/li&gt;&lt;li&gt;Rechtsverordnung&lt;/li&gt;&lt;li&gt;Verwaltungsverordnung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Verwaltungshandeln: Verordnung&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Verfassungsbegriff (Art. 139 B-VG)&lt;/li&gt;&lt;li&gt;Generelle (abstrakte oder konkrete) Anordnung einer Verwaltungsbehörde&lt;/li&gt;&lt;li&gt;Erst mit Kundmachung gültig&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Arten von Bescheiden&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Leistungsbescheid&lt;/strong&gt;: ordnet Tun oder Unterlassen an, &lt;strong&gt;vollstreckbar&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gestaltungsbescheid&lt;/strong&gt;: Gestaltet eine Rechtslage neu, &lt;strong&gt;nicht vollstreckbar&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Feststellungsbescheid&lt;/strong&gt;: verbindliche Feststellung einer unklaren Rechtslage, &lt;strong&gt;nicht vollstreckbar&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Formen des Verwaltungshandelns&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Bescheid&lt;/li&gt;&lt;li&gt;Verordnung&lt;/li&gt;&lt;li&gt;Maßnahme&lt;/li&gt;&lt;li&gt;Schlicht-hoheitliches Handeln&lt;/li&gt;&lt;li&gt;(Verwaltungsrechtlicher Vertrag)&lt;/li&gt;&lt;li&gt;Privatrechtliches Handeln&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Approbationsbefugnis&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Innerbehördliches Mandat&lt;/li&gt;&lt;li&gt;Organwalter kann Aufgaben an das Amt übertragen&lt;/li&gt;&lt;li&gt;Approbationsbefugte Beamte können damit "im Auftrag" der Behörde Bescheide oder Verordnungen erlassen, der Organwalter ist jedoch immer weisungsbefugt.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Amt&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Einer Behörde zugeordneter bürokratischer Hilfsapparat, handelt nicht selbst hoheitlich. &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Behörde&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Verwaltungsorgane mit Rechtssetzungsbefugnissen (handeln hoheitlich)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Verwaltungsaufgabe&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Staatliche Aufgabe der Verwaltung einer Gebietskörperschaft&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Staatliche Aufgabe&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Öffentliche Aufgabe, die der Gesetzgeber dem Staat zuweist&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Aufgabe&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Organisation &lt;strong&gt;soll&lt;/strong&gt; in einer Sache handeln&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Pflichtaufgabe: muss Handeln&lt;/li&gt;&lt;li class="ql-indent-1"&gt;öffentliche Aufgabe: im Interesse der Allgemeinheit&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Zuständigkeit&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Die &lt;strong&gt;Möglichkeit&lt;/strong&gt; einer Organisation in einer Sache zu handeln&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Organwalter (Definition, Zuordnung, Arten)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Den abstrakten Organen werden konkrete Menschen zugeordnet. &lt;/li&gt;&lt;li&gt;Gesetzessprache verwendet Organ und Organwalter oft synonym&lt;/li&gt;&lt;li&gt;Immer einer Gebietskörperschaft zugeordnet&lt;/li&gt;&lt;li&gt;Arten (Gesamtbegriff &lt;strong&gt;öffentliche Bedienstete&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Beamte = ernannte berufsmäßige Organe&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vertragsbedienstete = vertraglich bestellte Organe&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Organisation&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Abstrakte Konstrukte der Rechtsordnung denen bestimmte Aufgaben zukommen, bestehen meist aus vielen Organen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;z.B.: Gebietskörperschaft, Verwaltungsorganisation, Gerichtsorganisation&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;3 Rechtsordnungen&lt;/p&gt;</t>
   </si>
   <si>
@@ -817,7 +937,7 @@
     <t>&lt;ul&gt;&lt;li&gt;Gegen zu hohe Staatsverschuldung&lt;/li&gt;&lt;li&gt;Nachhaltig geordnete Haushalte: ausgewogenes Wirtschaftswachstum, wettbewerbsfähige soziale Marktwirtschaft, Preisstabilität, hohes Beschäftigungsniveau und sozialer Fortschritt (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel13" rel="noopener noreferrer" target="_blank"&gt;Art. 13 Abs. 2 b-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Demokratie&lt;/p&gt;</t>
+    <t>&lt;p&gt;Demokratie in Österreich (gesetzl. Grundlage)&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;"Herrschaft des Volkes". &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel1" rel="noopener noreferrer" target="_blank"&gt;Art. 1 B-VG&lt;/a&gt;: "Österreich ist eine demokratische Republik. Ihr Recht geht vom Volk aus." (seit 1918); wichtigstes Grundprinzip der Verfassung;&lt;/p&gt;</t>
@@ -874,7 +994,7 @@
     <t>&lt;p&gt;Republik und Bundespräsident&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;von lat. res publica&lt;/p&gt;&lt;p&gt;Staatsoberhaupt: (Bundes)Präsident (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel60" rel="noopener noreferrer" target="_blank"&gt;Art. 60ff B-VG&lt;/a&gt;)&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Vom Volk gewählt&lt;/li&gt;&lt;li&gt;Dem Volk verantwortlich&lt;/li&gt;&lt;li&gt;Funktionsperiode: 2x 6 Jahre&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;von lat. res publica&lt;/p&gt;&lt;p&gt;Österreich ist eine demokratische Republik (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel1" rel="noopener noreferrer" target="_blank"&gt;Art. 1 B-VG&lt;/a&gt;)&lt;/p&gt;&lt;p&gt;Staatsoberhaupt: (Bundes)Präsident (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel60" rel="noopener noreferrer" target="_blank"&gt;Art. 60ff B-VG&lt;/a&gt;)&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Vom Volk gewählt&lt;/li&gt;&lt;li&gt;Dem Volk verantwortlich&lt;/li&gt;&lt;li&gt;Funktionsperiode: 2x 6 Jahre&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Unterscheidung von Rechtsnormen&lt;/p&gt;</t>
@@ -958,7 +1078,7 @@
     <t>&lt;p&gt;Justizverwaltung&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Handlungen außerhalb der rechtsprechenden Tätigkeit&lt;/li&gt;&lt;li&gt;Organisatorisches Umfeld der Richter&lt;/li&gt;&lt;li&gt;= weisungs&lt;strong&gt;abhängige&lt;/strong&gt; Vollziehung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ausnahme: Verwaltung die (durch das Gesetz) Richtersenaten oder Kommissionen zugewiesen sind, diese sind weisungsfrei.&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;Handlungen außerhalb der rechtsprechenden Tätigkeit&lt;/li&gt;&lt;li&gt;Organisatorisches Umfeld der Richter&lt;/li&gt;&lt;li&gt;= weisungs&lt;strong&gt;abhängige&lt;/strong&gt; Vollziehung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ausnahme: Verwaltung die (durch das Gesetz) Richtersenaten oder Kommissionen zugewiesen sind, diese sind weisungsfrei (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel87" rel="noopener noreferrer" target="_blank"&gt;Art. 87 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Verbot wechselseitiger Instanzenzüge&lt;/p&gt;</t>
@@ -1210,7 +1330,7 @@
     <t>&lt;p&gt;Bundesrat &lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;(Zweck, Leitung, Legislaturperiode, Auflösung, Mitglieder)&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Erlaubt Ländern an Bundesgesetzgebung mitzuwirken&lt;/li&gt;&lt;li&gt;Hat Präsident (wechselt halbjährlich zwischen Ländern) und 2 Vizepräsidenten (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel36" rel="noopener noreferrer" target="_blank"&gt;Art. 36 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Bei Landtagswahl sendet der Landtag Mitglieder in den BR, BR hat keine Legislaturperiode, sondern wird stetig partiell erneuert.&lt;/li&gt;&lt;li&gt;Wird nicht aufgelöst, weil keine Legislaturperiode&lt;/li&gt;&lt;li&gt;61 Mitglieder (Bundesräte), g&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;rößtes Bundesland 12, Rest&lt;/span&gt; im Verhältnis zur Bürgerzahl, mindestens 3&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;Erlaubt Ländern an Bundesgesetzgebung mitzuwirken&lt;/li&gt;&lt;li&gt;Hat Präsident (wechselt halbjährlich zwischen Ländern) und 2 Vizepräsidenten (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel36" rel="noopener noreferrer" target="_blank"&gt;Art. 36 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Bei Landtagswahl sendet der Landtag Mitglieder in den BR, BR hat keine Legislaturperiode, sondern wird stetig partiell erneuert. &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel35" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;Art. 35 Abs. 1 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Wird nicht aufgelöst, weil keine Legislaturperiode&lt;/li&gt;&lt;li&gt;61 Mitglieder (Bundesräte), g&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;rößtes Bundesland 12, Rest&lt;/span&gt; im Verhältnis zur Bürgerzahl, mindestens 3 &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel34" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;Art. 34 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Schlichte Parlamentsbeschlüsse&lt;/p&gt;</t>
@@ -1282,7 +1402,7 @@
     <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Bundesgesetzgebung: Kundmachung&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Abschluss des Gesetzgebungsverfahren&lt;/li&gt;&lt;li&gt;BK gibt Gesetze im Bundesgesetzblatt elektronisch kund&lt;/li&gt;&lt;li&gt;Geregelt in Bundesgesetzblattgesetz&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel49" rel="noopener noreferrer" target="_blank"&gt;Art. 49 B-VG&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Abschluss des Gesetzgebungsverfahren&lt;/li&gt;&lt;li&gt;BK gibt Gesetze im Bundesgesetzblatt elektronisch kund&lt;/li&gt;&lt;li&gt;Geregelt in Bundesgesetzblattgesetz&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Legisvakanz&lt;/p&gt;</t>
@@ -1342,13 +1462,13 @@
     <t>&lt;p&gt;Inkompatibilität der Ämter&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Bestimmte Ämter können neben&lt;/p&gt;&lt;ul&gt;&lt;li&gt;d&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;em Mandat &lt;/span&gt;eines allgemeinen Vertretungskörpers&lt;/li&gt;&lt;li&gt;Mitglied des EU Parlaments&lt;/li&gt;&lt;li&gt;Mitglied der Regierung&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;nicht ausgeübt werden.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;NR, BR und EU-Parlament schließen sich aus (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel59" rel="noopener noreferrer" target="_blank"&gt;Art. 59 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Mandatar eines allg. Vertretungskörpers darf nicht &lt;strong&gt;BP &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel61" rel="noopener noreferrer" target="_blank"&gt;Art. 61 Abs. 1 iVm&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel23" rel="noopener noreferrer" target="_blank"&gt;Art. 23b Abs. 3 B-VG&lt;/a&gt;), &lt;strong&gt;Rechnungshofpräsident &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel122" rel="noopener noreferrer" target="_blank"&gt;Art. 122 Abs. 5 B-VG&lt;/a&gt;), &lt;strong&gt;Volksanwalt &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel148" rel="noopener noreferrer" target="_blank"&gt;Art. 148g Abs. 5 B-VG&lt;/a&gt;) sein&lt;/li&gt;&lt;li&gt;Mitglied der Bundes/Landesregierung darf nicht Volksanwalt sein&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Mandatar eines allg. Vertretungskörpers bzw. Regierungsmitglieder dürfen nicht &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Richter &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;am &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;OGH &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel92" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Art. 92 Abs. 2 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;), bei einem &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;VwG &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;oder &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;VwGH &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel134" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Art. 134 Abs. 5 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;) oder &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;VfGH &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel147" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Art. 147 Abs. 4 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;Bestimmte Ämter können neben&lt;/p&gt;&lt;ul&gt;&lt;li&gt;d&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;em Mandat &lt;/span&gt;eines allgemeinen Vertretungskörpers&lt;/li&gt;&lt;li&gt;Mitglied des EU Parlaments&lt;/li&gt;&lt;li&gt;Mitglied der Regierung&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;nicht ausgeübt werden.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;NR, BR und EU-Parlament schließen sich aus (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel59" rel="noopener noreferrer" target="_blank"&gt;Art. 59 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Mandatar eines allg. Vertretungskörpers darf nicht &lt;strong&gt;BP &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel61" rel="noopener noreferrer" target="_blank"&gt;Art. 61 Abs. 1 iVm&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel23b" rel="noopener noreferrer" target="_blank"&gt;Art. 23b Abs. 3 B-VG&lt;/a&gt;), &lt;strong&gt;Rechnungshofpräsident &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel122" rel="noopener noreferrer" target="_blank"&gt;Art. 122 Abs. 5 B-VG&lt;/a&gt;), &lt;strong&gt;Volksanwalt &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel148g" rel="noopener noreferrer" target="_blank"&gt;Art. 148g Abs. 5 B-VG&lt;/a&gt;) sein&lt;/li&gt;&lt;li&gt;Mitglied der Bundes/Landesregierung darf nicht &lt;strong&gt;Volksanwalt &lt;/strong&gt;sein &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel148g" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(105, 122, 180);"&gt;Art. 148g Abs. 5 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;) &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Mandatar eines allg. Vertretungskörpers bzw. Regierungsmitglieder dürfen nicht &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Richter &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;am &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;OGH &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel92" rel="noopener noreferrer" target="_blank" style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Art. 92 Abs. 2 B-VG&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;), bei einem &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;VwG &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;oder &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;VwGH &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel134" rel="noopener noreferrer" target="_blank" style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Art. 134 Abs. 5 B-VG&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;) oder &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;VfGH &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel147" rel="noopener noreferrer" target="_blank" style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Art. 147 Abs. 4 B-VG&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Landtag (Wahl, Auflösung, Abgeordnetenrechte und Einschränkungen, Tätigkeit)&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;5-6 Jährige Legislaturperiode&lt;/li&gt;&lt;li&gt;Wahl&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Von Landesbürger gewählt (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel6" rel="noopener noreferrer" target="_blank"&gt;Art. 6 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gleiche Wahlrechtsgrundsätze wie NR (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel595" rel="noopener noreferrer" target="_blank"&gt;Art. 95 Abs. 1 B-VG&lt;/a&gt;);&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Land darf Alter herab, aber nicht hinauf setzen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel95" rel="noopener noreferrer" target="_blank"&gt;Art. 95 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;BP kann Landtag auf Vorschlag der Bundesregierung mit Zustimmung des BR auflösen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel100" rel="noopener noreferrer" target="_blank"&gt;Art. 100 Abs. 1 B-VG&lt;/a&gt;) oder Selbstauflösung&lt;/li&gt;&lt;li&gt;freies Mandat, Immunität, Inkompatibilität wie bei NR&lt;/li&gt;&lt;li&gt;B-VG enthält Grundsätze über Landesgesetzgebung, wird durch Landesgesetze genauer spezifiziert.&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;5-6 Jährige Legislaturperiode&lt;/li&gt;&lt;li&gt;Wahl&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Von Landesbürger gewählt (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel6" rel="noopener noreferrer" target="_blank"&gt;Art. 6 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gleiche Wahlrechtsgrundsätze wie NR (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel95" rel="noopener noreferrer" target="_blank"&gt;Art. 95 Abs. 1 B-VG&lt;/a&gt;);&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Land darf Alter herab, aber nicht hinauf setzen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel95" rel="noopener noreferrer" target="_blank"&gt;Art. 95 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;BP kann Landtag auf Vorschlag der Bundesregierung mit Zustimmung des BR auflösen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel100" rel="noopener noreferrer" target="_blank"&gt;Art. 100 Abs. 1 B-VG&lt;/a&gt;) oder Selbstauflösung&lt;/li&gt;&lt;li&gt;freies Mandat, Immunität, Inkompatibilität wie bei NR&lt;/li&gt;&lt;li&gt;B-VG enthält Grundsätze über Landesgesetzgebung, wird durch Landesgesetze genauer spezifiziert.&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Weg der Landesgesetzgebung&lt;/p&gt;</t>
@@ -1366,7 +1486,7 @@
     <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Bundespräsidenten&lt;/span&gt; und Gewaltenteilung&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Oberstes Organ der &lt;strong&gt;Verwaltung &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel19" rel="noopener noreferrer" target="_blank"&gt;Art. 19 Abs. 1 B-VG&lt;/a&gt;) aber &lt;strong&gt;nicht weisungsbefugt &lt;/strong&gt;(das ist nur die Regierung).&lt;/li&gt;&lt;li&gt;BP ernennt und entlässt Regierung&lt;/li&gt;&lt;li&gt;Verwaltungsapparat des BP: &lt;strong&gt;Präsidentschaftskanzlei&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Verwaltungsakte des BP: Entschließungen&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;Oberstes Organ der &lt;strong&gt;Verwaltung &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel19" rel="noopener noreferrer" target="_blank"&gt;Art. 19 Abs. 1 B-VG&lt;/a&gt;) aber &lt;strong&gt;nicht weisungsbefugt &lt;/strong&gt;(das ist nur die Regierung).&lt;/li&gt;&lt;li&gt;BP ernennt und entlässt Regierung&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Wahl des &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Bundespräsidenten&lt;/span&gt;&lt;/p&gt;</t>
@@ -1378,7 +1498,7 @@
     <t>&lt;p&gt;Absetzung des Bundespräsidenten&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Bundesversammlung (einfache Mehrheit) kann auf Initiative des NR (2/3 Mehrheit) eine Volksabstimmung anordnen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel60" rel="noopener noreferrer" target="_blank"&gt;Art. 60 Abs. 6 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Bundesversammlung kann BP (1/2 Präsenzquorum, 2/3 Konsensquorum)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bei Verletzung der Verfassung beim VfGH anklagen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel142" rel="noopener noreferrer" target="_blank"&gt;Art. 142 Abs. 2 lit. a B-VG&lt;/a&gt;) anklagen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Antrag auf Amtsverlust wenn BP Wählbarkeit verliert (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel141" rel="noopener noreferrer" target="_blank"&gt;Art. 141 Abs. 1 lit. d B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;Bundesversammlung (einfache Mehrheit) kann auf Initiative des NR (2/3 Mehrheit) eine Volksabstimmung anordnen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel60" rel="noopener noreferrer" target="_blank"&gt;Art. 60 Abs. 6 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Bundesversammlung kann BP (1/2 Präsenzquorum, 2/3 Konsensquorum)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bei Verletzung der Verfassung beim VfGH anklagen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel142" rel="noopener noreferrer" target="_blank"&gt;Art. 142 Abs. 2 lit. a B-VG&lt;/a&gt;) anklagen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Antrag auf Amtsverlust bei VfGH stellen, wenn BP Wählbarkeit verliert (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel141" rel="noopener noreferrer" target="_blank"&gt;Art. 141 Abs. 1 lit. d B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Bundespräsident: Bildung der Bundesregierung und Landesregierung &lt;/span&gt;&lt;/p&gt;</t>
@@ -1780,7 +1900,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B230"/>
+  <dimension ref="A1:B250"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -3626,6 +3746,166 @@
         <v>459</v>
       </c>
     </row>
+    <row r="231" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Add cards for Gemeindeverwaltung
Closes #16
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - KS Oeffentliches Recht I (JKU, Austria).xlsx
+++ b/flashcards/Memcode - KS Oeffentliches Recht I (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="534">
   <si>
     <t>Question</t>
   </si>
@@ -19,748 +19,850 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Wann ist die Zustimmung der Bundesregierung für ein Landesgesetz notwendig? Wie wird die Zustimmung eingeholt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Bundesorgane sollen bei Vollziehung mitwirken (&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel97" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Art. 97 Abs. 2 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Ein eigenes Statut (Stadtrecht) ist betroffen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 116 Abs. 3 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Änderung der Organisation der Behörden der allg. staatlichen Verwaltung in den Ländern (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel15" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 15 Abs. 10 B-VG)&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Der LH muss vor Kundmachung dem Bundeskanzleramt bekannt das Gesetz geben. Regierung hat 8 Wochen für Ablehnung&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Organe einer Einheitsgemeinde? Was sind die Ämter dafür?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel117" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;Art. 117 Abs. 1 B-VG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Gemeinderat&lt;/li&gt;&lt;li&gt;Gemeindevorstand (Stadtrat)&lt;/li&gt;&lt;li&gt;Bürgermeister&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Für alle 3: Das Gemeindeamt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche zusätzliche Funktion hat der Bürgermeister von Wien? Was bedeutet das für die Wahl?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Er ist auch Landeshauptmann&lt;/li&gt;&lt;li&gt;Eine Direktwahl durch das Volk ist nicht möglich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche 3 Verwaltungsrollen hat die Stadt Wien?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wien ist Gemeinde, Statutarstadt und Bundesland&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Besonderheiten der Bezirksverwaltung durch eine Statutarstadt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;Art. 116 Abs. 3 B-VG&lt;/a&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ist keine Selbstverwaltung&lt;/li&gt;&lt;li&gt;Gebunden an Weisungen der Verwaltungsorgane von Bund und Land&lt;/li&gt;&lt;li&gt;Ist ein übertragener Wirkungsbereich: Wird von Bürgermeister besorgt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was bedeutet Einheitsgemeinde?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Alle Gemeinden, außer Statutarstädte, haben einen im Umfang einheitlichen Wirkungsbereich und ein einheitliches Organisationsrecht. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Gebietsgemeinde?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Auch für Überörtliche Angelegenheiten zuständig&lt;/li&gt;&lt;li&gt;Überörtlicher Selbstverwaltungskörper&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine Ortsgemeinde?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Für örtliche Angelegenheiten zuständig&lt;/li&gt;&lt;li&gt;Selbstverwaltungskörper&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der übertragene Wirkungsbereich von Gemeinden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Landes- und Bundesgesetzgebung können Zuständigkeiten an die Gemeinden übertragen, dies werden vom Bürgermeister besorgt.&lt;/li&gt;&lt;li&gt;Für diese ist die Gemeinde an Landes- oder Bundesverwaltung weisungsgebunden.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer hat die Rechtsaufsicht über Gemeinden bei welchen Angelegenheiten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Art. 10 B-VG: die Behörden der allgemeinen staatlichen Verwaltung des Bundes.&lt;/p&gt;&lt;p&gt;Art. 11, 12, 15 B-VG: d&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;ie Behörden der allgemeinen staatlichen Verwaltung des Landes.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsaufsicht der Staaten über die Gemeinden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die staatliche Verwaltung darf keine Weisungen erteilen, überprüft aber das Gemeindehandeln auf &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Gesetzeswidrigkeit &lt;/span&gt;und schreitet bei Übertretungen ein. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gemeinden sind Weisungsfrei. Was bedeutet das innerhalb der Gemeinde?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Innerhalb der Gemeinde herrscht Weisungsbindung. &lt;/li&gt;&lt;li&gt;Der Gemeinderat ist gegenüber den anderen Organen weisungsberechtigt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer wählt die Gemeinde(verwaltungs)organe&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Unmittelbar das Gemeindevolk (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel117" rel="noopener noreferrer" target="_blank"&gt;Art. 117 Abs. 2,6 B-VG&lt;/a&gt;) (Sonst: Verwaltungsorgane nicht vom Volk gewählt)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wem sind die Organe der Gemeinde politisch Verantwortlich?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Den Gemeindebürgern, &lt;strong&gt;nicht&lt;/strong&gt; den obersten Verwaltungsorganen&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Darf die staatliche Verwaltung den Gemeinden Weisungen erteilen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein, die Gemeinden sind autonom.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;In welchen Artikeln werden Gemeindeverwaltungsangelegenheiten geregelt? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel115" rel="noopener noreferrer" target="_blank"&gt;Art. 115ff B-VG&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Hat die Gemeinde Gesetzgebende oder richterliche Zuständigkeiten&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein, sie ist eine Verwaltungsorganisation&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine formalgesetzliche Delegation?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ein Gesetz bestimmt das Handeln der Vollziehung nicht oder nur sehr ungenau, dies ist verfassungswidrig (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel18" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(105, 122, 180);"&gt;Art 18. Abs 1. B-VG&lt;/a&gt;). Der Gesetzgeber delegiert daher die Pflicht das Recht zu bestimmen an die Vollziehung.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Landesverwaltung: Landesregierung (Zuständigkeit, Zusammensetzung, Entscheidungsfindung, Wahl, Regierungsart, Amt)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Oberstes Organ der Landesverwaltung, zuständig für hoheitliche (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel11" rel="noopener noreferrer" target="_blank"&gt;Art. 11-15 B-VG&lt;/a&gt;) und nicht hoheitliche (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel17" rel="noopener noreferrer" target="_blank"&gt;Art. 17 B-VG&lt;/a&gt;) Verwaltung&lt;/li&gt;&lt;li&gt;Besteht aus Landeshauptmann und weiteren Landesräten (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel101" rel="noopener noreferrer" target="_blank"&gt;Art. 101 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Entscheidet als Kollegialorgan, Landesräte können teilweise auch als Einzelorgane tätig werden (Ämter der Landesregierungen)&lt;/li&gt;&lt;li&gt;Parlamentarisches System: Landtag wählt Regierung &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel101" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;Art. 101 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Meist Mehrheitsregierung, außer in OÖ, NÖ und W → Proporzregierung=Konzentrationsregierung&lt;/li&gt;&lt;li&gt;Amt der Landesregierung: Hilfsapparat der Regierung &lt;strong&gt;&lt;em&gt;und &lt;/em&gt;&lt;/strong&gt;des Landeshauptmanns.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Grundrechtsquellen: Grundrechte im B-VG&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gleichheitssatz (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel7" rel="noopener noreferrer" target="_blank"&gt;Art. 7 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Recht auf den gesetzlichen Richter (&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel83" rel="noopener noreferrer" target="_blank" style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Art. 83 Abs. 2 B-VG&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Recht der Richter auf Unabhängigkeit (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel87" rel="noopener noreferrer" target="_blank"&gt;Art. 87 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Recht der Gemeinden auf Selbstverwaltung (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank"&gt;Art. 116 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Weisungsfreie Vollziehung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Unabhängige &lt;strong&gt;Richter &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel87" rel="noopener noreferrer" target="_blank"&gt;Art. 87 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;weisungsfreier Teil der &lt;strong&gt;Justizverwaltung &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel87" rel="noopener noreferrer" target="_blank"&gt;Art. 87 Abs. 2 B-VG&lt;/a&gt;): Richtersenate und Kommissionen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gemeindeselbstverwaltung&lt;/strong&gt;: Gemeinderat und Bürgermeister (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;Art. 116 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Weisungsfrei, unterliegen nur Aufsicht der Bundes/Landesbehörden.&lt;/li&gt;&lt;li&gt;Einfacher Bundes/Landesgesetzgeber kann weitere Verwaltungsorgane bei Rechtfertigung weisungsfrei stellen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel20" rel="noopener noreferrer" target="_blank"&gt;Art. 20 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie regelt die (Finanz)Verfassung wie der Staat zu seinem Geld kommt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Konstruiert den Staat als Abgabestaat&lt;/li&gt;&lt;li&gt;Staat bringt das Geld zwangsweise durch hoheitliche Abgaben, Gebühren und Beiträge auf.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie wird das Budget bestimmt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In einem Budgetgesetz (Bundesfinanzgesetz) auf der Grundlage eines Bundesfinanzrahmengesetzes&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie nennt man das Geld- und Vermögensrelevante Handeln der Verwaltung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gebarung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wo liegt die Budgethoheit, was bedeutet sie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Beim Parlament, das Parlament entscheidet, wofür die Verwaltung welche Summen ausgeben darf. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sind Gemeinden unter dem Grundrechtsschutz?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ja, die Gemeindeautonomie (Recht auf Selbstverwaltung, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank"&gt;Art. 116 Abs. 1 B-VG&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer ist ausgenommen aus dem Grundrechtsschutz?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Staaten (Bund und Land), die Grundrechte sind nicht dazu da den Staat vor sich selbst, Land vor dem Bund oder Bund vor dem Land zu schützen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Können Gebietskörperschaften Träger von Grundrechten sein?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ja, juristische Personen&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (des öffentlichen und des Privatrechts)&lt;/span&gt; können Träger von Grundrechten sein, wenn dies &lt;strong&gt;wesensmäßig &lt;/strong&gt;möglich ist.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gilt der Gleichheitssatz auch für die nicht-hoheitliche Verwaltung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ja, Diskriminierung ist verboten, und Sachlichkeit wird verlangt. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Fiskalgeltung der Grundrechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Bindung des Staates an die Grundrechte im Rahmen der Privatwirtschaftsverwaltung.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Verwaltung kann sowohl hoheitlich als auch privatrechtlich Handeln. Gilt der Grundrechtsschutz auch gegen die nicht-hoheitlichen Handlungen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ja&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie nennt man Verwaltungsakte des BP?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Entschließungen&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Verwaltungsapparat des BP?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Präsidentschaftskanzl&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;ei&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sicherheitsverwaltung: Was is das Bundesheer? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;militärische Formation des Bundes, zählt zur unmittelbaren Bundesverwaltung&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sicherheitsbehörden des Bundes&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78a" rel="noopener noreferrer" target="_blank"&gt;Art. 78a-c B-VG&lt;/a&gt; richten die Sicherheitsbehörden ein&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/spg/paragraf/2" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;2 Abs. 2 SPG&lt;/a&gt; definiert Aufgaben der Sicherheitsverwaltung&lt;/li&gt;&lt;li&gt;2/3 Ebenen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;BM für Inneres&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Landespolizeidirektion&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bezirksverwaltungsbehörde&lt;/li&gt;&lt;li&gt;Mischform aus mittelbarer und unmittelbarer Bundesverwaltung, weil auf unterer Ebene teilweise Bezirksverwaltungsbehörden als Landesbehörden eingebunden sind&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;Durchführungsverordnung &lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Präzisiert ein Gesetz (&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel18" rel="noopener noreferrer" target="_blank" style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Art. 18 Abs. 2 B-VG&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;)&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kompetenzverteilung in der nicht-hoheitlichen Verwaltung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel17" rel="noopener noreferrer" target="_blank"&gt;Art. 17 B-VG&lt;/a&gt;: Kompetenzverteilung in Art. 10 - 15 B-VG gilt &lt;strong&gt;nicht&lt;/strong&gt; für nicht-hoheitliche Verwaltung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das hoheitliche Organisationsrecht einer Gebietskörperschaft?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Bestimmt die innere Willensbildung des &lt;strong&gt;privatrechtlichen&lt;/strong&gt; Handelns&lt;/li&gt;&lt;li&gt;Zuständigkeit für Kaufverträge, Willensbildung, inhaltliche Gestaltung von Verträgen ⇾ bestimmt das hoheitliche Organisationsrecht (nicht die Privatrechtsordnung)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie funktioniert das Gesetzmäßigkeitsgebot in der nicht-hoheitlichen Verwaltung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Geregelt durch das Verwaltungsprivatrecht&lt;/li&gt;&lt;li&gt;&lt;strong&gt;differenziertes Legalitätsprinzip: &lt;/strong&gt;Auch privatrechtliche Handlungen unterliegen dem Gesetzmäßigkeitsgebot,  es ist aber flexibler und weniger streng, als für hoheitliches Handeln &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Inhalt der nicht-hoheitlichen Verwaltung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Privatwirtschaftsverwaltung&lt;/li&gt;&lt;li&gt;Fiskalverwaltung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer kann nicht-hoheitlich handeln, wer nicht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Nur die juristischen Personen: Bund, Länder und Gemeinden, also nur die Verwaltung. &lt;/li&gt;&lt;li&gt;Parlamente und Gerichte handeln  immer hoheitlich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Gebietskörperschaften sind Träger von Privatrechten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel17" rel="noopener noreferrer" target="_blank"&gt;Art. 17 B-VG&lt;/a&gt;: Bund und Länder sind juristische Personen&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank"&gt;Art. 116 Abs. 2 B-VG&lt;/a&gt;: Gemeinden sind juristische Personen&lt;/li&gt;&lt;li&gt;Vermögensfähig sind also der Bund, die Länder und die Gemeinden, nicht der Gesamtstaat Österreich.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Unterschiede zwischen juristischen Personen des Privatrechts und des öffentlichen Rechts? Was ist identisch? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Unterschiede:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Privatrecht: Durch Vertrag errichtet&lt;/li&gt;&lt;li class="ql-indent-1"&gt;öffentliches Recht: Durch Gesetz errichtet&lt;/li&gt;&lt;li&gt;Beide haben dieselbe (Privat)Rechtsfähigkeit, dieselben privaten Rechte und Pflichten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist ein Organisationsrecht? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Regelt welche Organe eine juristische Person hat, und welche Organwalter für die jur. Person handeln.&lt;/li&gt;&lt;li&gt;Insbesondere wer intern entscheidet, und wer nach außen vertritt.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Jur. Person handelt immer nur durch vertretungsbefugte Organe.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die zwei Kernaussagen der Wesenstheorie?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Umfang der Rechte von jur. Personen im wesentlichen auf &lt;strong&gt;Vermögensrechte &lt;/strong&gt;beschränkt = &lt;strong&gt;Vermögensfähigkeit&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Jur. Personen sind rechtsfähig, benötigen aber Menschen um für sie zu handeln (&lt;strong&gt;Organisationsrecht&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Können juristische Personen Rechtsträger sein? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Privatrechtsordnung erlaubt, dass juristische Personen von der Rechtsordnung als Rechtsträger behandelt wären, als wären sie Menschen.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind juristische Personen? &lt;/p&gt;&lt;p&gt;Wie werden sie noch genannt?&lt;/p&gt;&lt;p&gt;Wie wird entschieden, welche juristischen Personen es gibt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;= virtuelle Menschen&lt;/li&gt;&lt;li&gt;Auch Rechtsperson oder Körperschaft genannt&lt;/li&gt;&lt;li&gt;Gesetzgebung entscheidet ob und welche juristischen Personen es gibt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind natürliche Personen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;= Menschen&lt;/li&gt;&lt;li&gt;Träger von Rechten und Pflichten&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;ABGB&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Allgemeines bürgerliches Gesetzbuch&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer ist der gesetzliche Vertreter für ein Kind?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Eltern (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/167" rel="noopener noreferrer" target="_blank"&gt;§ 167 ABGB&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ist jeder Mensch handlungsfähig?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/21" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;21 ABGB&lt;/a&gt;), wer nicht handlungsfähig ist, braucht einen Vertreter der für ihn handelt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Handlungsfähigkeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die Fähigkeit, durch eigenes Handeln Rechte zu erwerben und Pflichten zu begründen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Rechtsfähigkeit? Wer hat sie wie lange? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die Fähigkeit, Träger privater Rechte und Pflichten zu sein (z.B.: Eigentümer von Geld und Vermögen)&lt;/li&gt;&lt;li&gt;Jeder Mensch ist von Geburt bis zum Tod rechtsfähig.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Einzelne Grundrechte&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eigentumsfreiheit&lt;/li&gt;&lt;li&gt;Erwerbsfreiheit&lt;/li&gt;&lt;li&gt;Recht auf persönliche Freiheit&lt;/li&gt;&lt;li&gt;Hausrecht&lt;/li&gt;&lt;li&gt;Versammlungsfreiheit&lt;/li&gt;&lt;li&gt;Meinungsfreiheit&lt;/li&gt;&lt;li&gt;...&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Recht auf den gesetzlichen Richter?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(102, 102, 102);"&gt; Justizgrundrecht, das festlegt, dass für Rechtsstreitigkeiten und Prozesse bereits im Voraus bestimmt sein muss, welches&amp;nbsp;&lt;/span&gt;Gericht&amp;nbsp;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(102, 102, 102);"&gt;und welcher Richter zuständig ist (&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel83" rel="noopener noreferrer" target="_blank"&gt;Art.&amp;nbsp;83 Abs. 2&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel87" rel="noopener noreferrer" target="_blank"&gt;Art. 87 Abs. 3&amp;nbsp;B-VG&lt;/a&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(102, 102, 102);"&gt;)&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Verfahrensgrundrechte&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Wehren den Staat nicht ab, sondern verlangen Einhaltung der durch die Verfassung gewährleisteten Verfahrensrechte &lt;/li&gt;&lt;li&gt;Beispiele: Recht auf den gesetzlichen Richter, Recht auf faires Verfahren, keine Strafe ohne Gesetz.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Politische Grundrechte (= Teilhaberechte)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Durch die Verfassung gewährleistete Recht der Teilnahme der Menschen am Staat&lt;/li&gt;&lt;li&gt;Keine Abwehrrechte, sondern Teilhaberechte (status activus)&lt;/li&gt;&lt;li&gt;Aktive Teilhabe an der Staatswillensbildung und Staatsgewalt&lt;/li&gt;&lt;li&gt;Beispiele: Wahlrecht, Recht auf Volksbegehren, Petitionsrecht, Gründung und Betätigungsfreiheit polit. Parteien.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Soziale Grundrechte&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Österreich ist ein Sozialstaat, die Verfassung kennt aber &lt;strong&gt;keine&lt;/strong&gt; sozialen Grundrechte.&lt;/li&gt;&lt;li&gt;Begründung: könnten den Staat wirtschaftlich überfordern.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Freiheitsrechte mit staatlichen Schutzpflichten&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Nicht nur Abwehrrecht gegen Staat&lt;/li&gt;&lt;li&gt;Anspruch gegen den Staat, dass er den Freiraum auch vor Beschädigung durch andere Privatpersonen schützt&lt;/li&gt;&lt;li&gt;Beispiele: Recht auf Leben (Art. 2 EMRK), Verbot der Folter, ..&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Freiheitsrechte ohne Gesetzesvorbehalt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Absolut schützendes Freiheitsrecht&lt;/li&gt;&lt;li&gt;Kein Eingriff in den Schutzbereich durch einfache Gesetze zulässig&lt;/li&gt;&lt;li&gt;Beispiele: Verbot der Folter, Verbot der Todesstrafe, ... &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die Organe einer Statutarstadt? Was sind die Ämter dafür?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gemeinderat&lt;/li&gt;&lt;li&gt;Stadtsenat&lt;/li&gt;&lt;li&gt;Bürgermeister&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Amt für alle 3: Magistrat&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Quoren für Landesverfassungsgesetze?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Präsenz 1/2, Konsens 2/3 (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel99" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 99 Abs. 2 B-VG&lt;/a&gt;)&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Arten der Leitung der Verwaltung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Aufsicht: &lt;/strong&gt;ex post - nach der Handlung&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Rechtsaufsicht: gesetzmäßig&lt;/li&gt;&lt;li&gt;Zweckaufsicht: zweckmäßig&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Weisung: &lt;/strong&gt;ex ante - vor der Handlung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Verwaltungshandeln: Bescheid&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Verfassungsbegriff (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel130" rel="noopener noreferrer" target="_blank"&gt;Art. 130 Abs. 1 B-VG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel132" rel="noopener noreferrer" target="_blank"&gt;Art. 132 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;3 formale Merkmale (nicht vorhanden: Absolut nichtig)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es muss eine Verwaltungsbehörde handeln&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es muss an einen individuellen Adressaten gerichtet sein&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es muss eine behördliche Anordnung enthalten&lt;/li&gt;&lt;li&gt;Gesetzgeber kann weitere Merkmale hinzufügen, Auswirkung des Fehlens legt Gesetzgeber fest (z.B.: relativ nichtig)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Eingriffsvorbehalt vs. Ausgestaltungsvorbehalt bei Freiheitsrechten&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Eingriffsvorbehalt &lt;/strong&gt;erlaubt in den Schutzbereich des Freiheitsrechts einzugreifen, und diesen durch Gesetz einzuschränken&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ausgestaltungsvorbehalt &lt;/strong&gt;erlaubt  nur ein Freiheitsrecht näher auszugestalten, nicht in den Schutzbereich einzugreifen.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was besagt die Wesensgehaltssperre?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ein Freiheitsrecht darf durch einen gesetzlichen Eingriff nicht hinfällig werden, ein Minimum an Freiheit muss bestehen bleiben.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Wie muss der Gesetzgeber handeln, wenn der Verfassungstext keine Vorgaben für einen gesetzlichen Eingriff auf ein Freiheitsrecht hat? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Es wird die Auslegung herangezogen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Gesetzgeber muss nachweislich ein konkretes öffentliches Interesse verfolgen&lt;/li&gt;&lt;li&gt;Der Eingriff muss verhältnismäßig sein (Verhältnismäßigkeitsgrundsatz), die Belastung der Freiheit darf nicht höher sein, als zur Erreichung des öffentlichen Interesses unbedingt erforderlich&lt;/li&gt;&lt;li&gt;Eingriff muss sachlich sein&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Freiheitsrechte mit Gesetzesvorbehalt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Relativ schützendes&lt;/strong&gt; Freiheitsrecht&lt;/li&gt;&lt;li&gt;Eingriff in den Schutzbereich durch einfache Gesetze möglich - unter Beachtung der &lt;strong&gt;materiellen Eingriffsschranken&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Steht unter materiellem Gesetzesvorbehalt, weil der Gesetzgeber bei seinen Regelungen inhaltlich an Vorhaben der Verfassung gebunden ist.&lt;/li&gt;&lt;li&gt;Der Verfassungstext sagt, ob ein Grundrecht unter materiellem Gesetzesvorbehalt steht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Beispiele für Freiheitsrechte&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Eigentumsfreiheit&lt;/li&gt;&lt;li&gt;Erwerbsfreiheit&lt;/li&gt;&lt;li&gt;Kunstfreiheit&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Freiheitsrechte, warum heißen sie auch Abwehrrechte?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Grundrechte, durch welche die Verfassung den Menschen Freiräume gewährleistet.&lt;/li&gt;&lt;li&gt;Erlauben dem einzelnen verfassungswidrige Eingriffe des Staats in den geschützten Freiraum abzuwehren (über den dafür vorgesehenen besonderen Prozessweg) &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Schützt der Gleichheitssatz vor eingriffen in den Freiraum der Menschen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein, er ist kein Freiheitsrecht&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Willkürverbot, was ist Willkür?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gilt für die Vollziehung&lt;/li&gt;&lt;li&gt;Verbot willkürlicher Entscheidungen&lt;/li&gt;&lt;li&gt; Willkür liegt vor, wenn eine Behörde&lt;/li&gt;&lt;li class="ql-indent-1"&gt;eine Person absichtlich benachteiligt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ohne Rechtsgrundlage entscheidet&lt;/li&gt;&lt;li class="ql-indent-1"&gt;die Rechtslage verkennt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gravierende Verfahrensfehler begeht&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wen bindet der Gleichheitssatz, wen nicht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Bindet den:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;einfachen Bundesgesetzgeber&lt;/li&gt;&lt;li&gt;einfachen Landesgesetzgeber&lt;/li&gt;&lt;li&gt;Landesverfassungsgesetzgeber&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Bindet nicht:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bundesverfassungsgesetzgeber, weil der Gleichheitssatz bloß ein Bundesverfassungsgesetz ist. &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann verletzt ein einfaches Gesetz den Gleichheitssatz?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wenn es:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Unsachliche Differenzierungen vornimmt&lt;/strong&gt; (Gleiches ist gleich zu behandeln, soweit kein Grund für eine Ungleichbehandlung vorliegt)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gebotene Differenzierungen unterlässt&lt;/strong&gt; (Ungleiches darf nicht ohne Grund gleich behandelt werden)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Sachlich nicht gerechtfertigte Regelungen&lt;/strong&gt; trifft.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gleichheitsformel&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Eine Ungleichbehandlung ist &lt;strong&gt;gleichheitskonform&lt;/strong&gt;, wenn sie sachlich gerechtfertigt ist. Eine Ungleichbehandlung ist &lt;strong&gt;gleichheitswidrig&lt;/strong&gt;, wenn sie &lt;strong&gt;nicht &lt;/strong&gt;sachlich gerechtfertigt ist.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;(z.B.: Matura als Voraussetzung für Studium ist konform, da allgemeine Vorbildung notwendig ist, um sinnvoll zu studieren)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kann der Gesetzgeber ungleiches gleich behandeln?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nein, bei unterschieden im Tatsächlichen (z.B.: unterschiedliches Einkommen) muss der Gesetzgeber auch unterschiedliche Regelungen erlassen (Gebot &lt;strong&gt;sachlicher Differenzierung&lt;/strong&gt;) &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was bedeutet &lt;strong&gt;gleich&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gleiche Betroffenheit der Rechtsunterworfenen unter Berücksichtigung aller rechtlichen und tatsächlichen Wirkungen&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gleichheitsrechte&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gleichheitssatz: &lt;a href="https://www.jusline.at/gesetz/stgg/paragraf/artikel2" rel="noopener noreferrer" target="_blank"&gt;Art 2. StGG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel7" rel="noopener noreferrer" target="_blank"&gt;Art 7 Abs. 1 B-VG&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Recht auf Gleichbehandlung von Fremden untereinander&lt;/li&gt;&lt;li class="ql-indent-1"&gt;BVG über die Beseitigung aller Formen rassischer Diskriminierung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Kategorien/Arten von Grundrechten gibt es?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gleichheitsrechte (Gleichheitssatz)&lt;/li&gt;&lt;li&gt;Freiheitsrechte (= Abwehrrechte)&lt;/li&gt;&lt;li&gt;Soziale Grundrechte&lt;/li&gt;&lt;li&gt;Politische Grundrechte (= Teilhaberechte)&lt;/li&gt;&lt;li&gt;Verfahrensgrundrechte&lt;/li&gt;&lt;li&gt;Sonstige Grundrechte&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind verfassungsimmanente&amp;nbsp;Schranken? Was bedeuten Sie für Grundrechte? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Einschränkung des Schutzbereichs des Grundrechts durch andere Grundrechte und objektive Verfassungsbestimmungen.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Der Schutzbereich des Grundrechts geht daher nicht zwangsläufig so weit, wie die Formulierung des Textes erwarten lässt.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie wird mit Widersprüchen in Grundrechtsquellen umgegangen? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Dasselbe Grundrecht kann an verschiedenen Stellen der Verfassungsordnung verankert sein. Widersprüche sind nach den Regeln der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;Derogation &lt;/strong&gt;aufzulösen.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie unterteilt die Verfassung unter objektivem Recht gewährleistete Rechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nach Adressatenkreis in Staatsbürgerrechte und Menschenrechte&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Drittwirkung der Grundrechte&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Durch Trennung von Staat und Gesellschaft gibt es &lt;strong&gt;keine Drittwirkung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Grundrechte gelten nur gegen den Staat, nicht Mensch gegen Mensch&lt;/li&gt;&lt;li&gt;Ausnahmen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gesetzlich angeordnete Drittwirkungen (z.B.: Datenschutzgesetz)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Grundrechte mit staatlicher Schutzpflicht (Recht auf Leben)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Mittelbare Drittwirkung im Zivilrecht (Auslegung, Sittenklauseln)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wo werden über Verstöße gegen Grundrechte entschieden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;OGH&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wo werden in der Regel über Verstöße gegen subjektives Recht entschieden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;im VfGH&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie wird der Schutzbereich eines Grundrechts festgelegt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die Verfassung die ein Grundrecht normiert, legt den Schutzbereich mit dem Wortlaut des Verfassungstextes fest. Diese Begriffe sind allerdings auslegungsbedürftig (z.&amp;nbsp;B.: Eigentumsfreiheit hat den Schutzbereich "Eigentum")&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Grundrechtsquellen: Einzelne Grundrechte in Staatsverträgen&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Rechte der Minderheiten&lt;/li&gt;&lt;li&gt;Religionsfreiheit&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Grundrechtsquellen: Grundrechte in einfachen Gesetzen&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Recht auf Zivildienst&lt;/li&gt;&lt;li&gt;Recht auf Datenschutz&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Grundrechtsquellen&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Quellen:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Grundrechtskataloge&lt;/li&gt;&lt;li&gt;Grundrechtsgesetze&lt;/li&gt;&lt;li&gt;Grundrechte im B-VG&lt;/li&gt;&lt;li&gt;Grundrechte in einfachen Gesetzen&lt;/li&gt;&lt;li&gt;Einzelne Grundrechte in Staatsverträgen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Grundrechtsquellen: Grundrechtsgesetze&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Hausrechts Gesetz &lt;/li&gt;&lt;li&gt;Beschluss der provisorischen Nationalversammlung über die Aufhebung der Zensur 1918&lt;/li&gt;&lt;li&gt;PersFrG (Bundesverfassungsgesetz zum Schutz der persönlichen Freiheit)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Grundrechtsquellen: Grundrechtskataloge&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;StGG 1867&lt;/li&gt;&lt;li&gt;EMRK + ZP&lt;/li&gt;&lt;li&gt;BVG Kinderrechte&lt;/li&gt;&lt;li&gt;EU Grundrechtecharta&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gegen wen schützen Grundrechte, gegen wen nicht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Grundrechte schützen gegen Staat und Staatsgewalt&lt;/li&gt;&lt;li&gt;Schützen auch gegen den Gesetzgeber&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gegen einfachen Bundesgesetzgeber&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gegen Landesverfassungsgesetzgeber&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gegen einfachen Landesgesetzgeber&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gegen die staatl. Vollziehung (Verwaltung und Gerichtsbarkeit)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aber: &lt;/strong&gt;Bundesverfassungsgesetze können Grundrechte einschränken. (z.&amp;nbsp;B.: Wehrpflicht für Männer widerspricht dem Gleichheitssatz, ist aber durch B-VG diskriminierend festgelegt) &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Objektives Recht&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Mensch hat keinen durchsetzbaren Anspruch auf Einhaltung der Gesetze&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Subjektives Recht&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Grundrechte sind gegen den Staat durchsetzbare Individualrechte&lt;/li&gt;&lt;li&gt;Mensch hat Anspruch auf Einhaltung der Gesetze (Verwaltung, Gerichtsbarkeit, Gesetzgebung verfolgen Verletzung der Grundrechte)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Grundrechte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Alle den Menschen durch formelle Verfassungsgesetze gewährleistete Recht&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Geschichte der Grund- und Freiheitsrechte&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;1789&lt;/strong&gt;: Deklaration der Menschen- und Bürgerrechte&lt;/p&gt;&lt;p&gt;&lt;strong&gt;1867&lt;/strong&gt;: Staatsgrundgesetz (Dezemberverfassung) &lt;/p&gt;&lt;p&gt;&lt;strong&gt;1948&lt;/strong&gt;: Allgemeine Erklärung der Menschenrechte&lt;/p&gt;&lt;p&gt;&lt;strong&gt;1950&lt;/strong&gt;: Europäische Menschenrechtskonvention&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(34, 38, 74); color: rgb(238, 236, 246);"&gt;Wachkörper: &lt;/span&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Gemeindewachkörper &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel118" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 118 Abs. 8 B-VG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel118a" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 118a B-VG&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;Gemeinde&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Aufgaben im kommunalen Bereich&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(34, 38, 74); color: rgb(238, 236, 246);"&gt;Wachkörper: &lt;/span&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Justizwache &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stvg/paragraf/13a" rel="noopener noreferrer" target="_blank" style="color: rgb(105, 122, 180); background-color: rgb(40, 45, 88);"&gt;§&amp;nbsp;13a Strafvollzugsgesetz&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;﻿Bund&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Bewachung der Strafgefangenen&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(34, 38, 74); color: rgb(238, 236, 246);"&gt;Wachkörper: &lt;/span&gt;Bundespolizei&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel10" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(105, 122, 180);"&gt;Art. 10 Abs. 1 Z. 14 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;, &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78d" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(105, 122, 180);"&gt;Art 78d B-VG&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Bund&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Innere Sicherheit&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Unmittelbare Bundesverwaltung, BM für Inneres an der Spitze&lt;/li&gt;&lt;li&gt;im Bereich jeder Landespolizeidirektion sind Bezirkskommanden bzw. Stadtpolizeikommanden eingerichtet&lt;/li&gt;&lt;li&gt;Wachkörper Bundespolizei ist von Sicherheitsbehörden des Bundes zu unterscheiden!&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wachkörper&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Bewaffnete Formationen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78d" rel="noopener noreferrer" target="_blank"&gt;Art. 78d Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bundespolizei: &lt;strong&gt;Bund&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Justizwache: &lt;strong&gt;Bund&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gemeindewachkörper: &lt;strong&gt;Gemeinde&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Organisation und Führung der Bundespolizei und die Org. sonstiger Wachkörper (Ausnahme: Gemeindewachkörper) ist Bundessache&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Sicherheitsbehörden: &lt;/span&gt;Bezirksverwaltungsbehörde&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Bezirkshauptmannschaft/Bürgermeister besorgt prinzipiell Sicherheitsverwaltung auf Bundesebene&lt;/li&gt;&lt;li&gt;Als Verwaltungsbehörde aber nicht auf Sicherheitsaufgaben spezialisiert.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Sicherheitsbehörden: Landespolizeidirektion&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78b" rel="noopener noreferrer" target="_blank" style="color: rgb(105, 122, 180); background-color: rgba(0, 0, 0, 0);"&gt;Art. 78b Abs. 1 B-VG&lt;/a&gt;) für jedes Bundesland:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Landespolizeidirektor weisungsgebunden an BM&lt;/li&gt;&lt;li class="ql-indent-1"&gt;BM muss jede wichtige Weisung an den LH mitteilen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;BM kann Landespolizeidirektor nur mit Einvernehmen des LH bestellen&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78c" rel="noopener noreferrer" target="_blank"&gt;Art. 78c B-VG&lt;/a&gt; ermächtigt einfachen Bundesgesetzgeber die Landespolizeidirektion zur Sicherheitsbehörde 1. Instanz zu bestimmen, &lt;a href="https://www.jusline.at/gesetz/spg/paragraf/8" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;8 SPG&lt;/a&gt; legt dafür einige Gebiete fest.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sicherheitsbehörden: BM für Inneres&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78a" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 78a Abs. 1 B-VG&lt;/a&gt;): Generaldirektion für öffentliche Sicherheit sorgt für Sicherheitsverwaltung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;SPG&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sicherheitspolizeigesetz&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Abgabebehörden&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Auftragsverwaltung des Bundes: für nicht-hoheitliche Verwaltung ist theoretisch nur der BM zuständig (z.&amp;nbsp;B.: Bundesvermögen, Geschäfte des Bundes)&lt;/li&gt;&lt;li&gt;BM kann einzelne Geschäfte durch hoheitlichen Auftrag dem LH übertragen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel104" rel="noopener noreferrer" target="_blank"&gt;Art. 104 Abs. 2&lt;/a&gt;) &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Unmittelbare Bundesverwaltung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel102" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(105, 122, 180);"&gt;Art. 102 Abs. 2 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ausnahme&lt;/li&gt;&lt;li&gt;Bund erledigt Aufgaben durch eigene Bundesbehörden&lt;/li&gt;&lt;li&gt;Bund darf dennoch mittelbare Bundesverwaltung nutzen &lt;/li&gt;&lt;li&gt;Mit Zustimmung der Länder, darf Bund auch Materien regeln, die nicht in Art. 102 Abs. 2 stehen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel102" rel="noopener noreferrer" target="_blank"&gt;Art. 102 Abs. 4 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Mittelbare Bundesverwaltung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel102" rel="noopener noreferrer" target="_blank"&gt;Art. 102 Abs. 1 B-VG&lt;/a&gt;)&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Das oberste Organ ist ein BM (oder der BK), als funktionelles und organisatorisches Organ des Bundes&lt;/li&gt;&lt;li&gt;Das mittlere Organ ist der Landeshauptmann (als Einzelorgan). &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Organisatorisch ein Landesorgan, funktionell aber im Auftrag des Bundes&lt;/li&gt;&lt;li class="ql-indent-1"&gt;An Weisungen des BM gebunden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Amt: Amt der Landesregierung&lt;/li&gt;&lt;li&gt;Das untere Organ ist die Bezirksverwaltungsbehörde&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Organwalter (Bezirkshauptmann/Bürgermeister) an Weisung des LH gebunden (In Bundesverwaltung, sonst an Landesregierung)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Amt: Bezirkshauptmannschaft/Magistrat&lt;/li&gt;&lt;li&gt;Unterste Organe: Gemeindeorgane&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Staatssekretäre &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Werden zwar in Art. 19 B-VG als oberste Organe der Verwaltung genannt, sind jedoch BM unterstellt und weisungsgebunden (&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78" rel="noopener noreferrer" target="_blank" style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Art. 78 Abs. 3 B-VG&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Aufgabe ist Unterstützung und Vertretung des BM, sie sind nicht Teil der Bundesregierung&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ämter der Bundesregierung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Bundeskanzleramt für BK&lt;/li&gt;&lt;li&gt;Bundesministerien für die BM&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Bundesregierung: &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;BK, VK und BMs als Einzelorgane&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Oberste Organe der Verwaltung (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel19" rel="noopener noreferrer" target="_blank"&gt;Art. 19 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;BM für Finanzen und für Inneres sind in der Verfassung, andere werden durch Bundesministeriengesetz 1986 bestimmt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Bundesregierung &lt;/span&gt;als Kollegialorgan&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;= Ministerrat&lt;/li&gt;&lt;li&gt;Beschlüsse müssen einstimmig sein&lt;/li&gt;&lt;li&gt;Aufgabe sind Regierungsakte wie&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vorschläge an BP (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel67" rel="noopener noreferrer" target="_blank"&gt;Art. 67 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesetzesvorlagen an das Parlament (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel41" rel="noopener noreferrer" target="_blank"&gt;Art. 41 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vorschläge für Ernennung von Verfassungsrichtern (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel147" rel="noopener noreferrer" target="_blank"&gt;Art. 147 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Zusammensetzung der Bundesregierung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Besteht aus BK, Vizekanzler und Bundesministern (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel19" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 19 Abs. 1 B-VG&lt;/a&gt;,&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel69" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt; Art. 69 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Landesverwaltung unterhalb der Regierung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Landesverwaltung in Verwaltungssprengel territorial gegliedert&lt;/li&gt;&lt;li&gt;Land in Bezirke gegliedert, 2 Arten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bezirk&lt;/strong&gt;, der mehrere Gemeinden erfasst&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Statutarstadt&lt;/strong&gt;, die alleine ein Bezirk ist&lt;/li&gt;&lt;li&gt;Bezirksverwaltungsbehörden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bezirkshauptmann (monokratisch), Amt: Bezirkshauptmannschaft&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bürgermeister, Amt: Magistrat&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sicherheitsverwaltung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sicherheitsbehörden des Bundes (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78a" rel="noopener noreferrer" target="_blank"&gt;Art. 78a-c B-VG&lt;/a&gt;)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ortspolizei&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Örtliche Verwaltungspolizei und örtliche Sicherheitspolizei gemeinsam&lt;/li&gt;&lt;li&gt;bei gesetzlicher Lücke zur Beseitigung konkreter Gefahren und Missstände, wenn diese das "örtliche Gemeinschaftsleben" stören &lt;/li&gt;&lt;li&gt;Gemeinde darf gesetzesergänzende Verordnungen erlassen (ortspolizeiliche Verordnungen &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel118" rel="noopener noreferrer" target="_blank"&gt;Art. 118 Abs. 6 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Örtliche Sicherheitspolizei&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Aus dem Kompetenztatbestand ausgenommen → Aufteilung in überörtliche und örtliche Sicherheitspolizei&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Sicherheitspolizei&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel10" rel="noopener noreferrer" target="_blank" style="color: rgb(105, 122, 180); background-color: rgb(40, 45, 88);"&gt;Art. 10 Abs. 1 Z. 7 B-VG&lt;/a&gt; Aufrechterhaltung der öffentlichen Ruhe, Ordnung und Sicherheit (soweit keiner konkreten Sachmaterie zugewiesen)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Örtliche Verwaltungspolizei&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Alle in &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel10" rel="noopener noreferrer" target="_blank" style="color: rgb(105, 122, 180); background-color: rgb(40, 45, 88);"&gt;Art. 10-15 B-VG&lt;/a&gt; enthaltenen Angelegenheiten der Verwaltungspolizei, die im &lt;em&gt;örtlichen Interesse&lt;/em&gt; gelegen sind, fallen in den Wirkungsbereich der Gemeinden&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Verwaltungspolizei&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Staatliches Handeln zur Abwehr und Beseitigung konkreter Gefahren und Missstände&lt;/li&gt;&lt;li&gt;Annexmaterie zu den Kompetenzen in &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel10" rel="noopener noreferrer" target="_blank"&gt;Art. 10-15 B-VG&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Allgemeine staatliche Verwaltung (Aufstellung in Bund und Ländern)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Allzuständigkeit der Staatsgewalt, erledigt von allgemeinen staatlichen Verwaltungsorganen&lt;/li&gt;&lt;li&gt;der Länder: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bezirksverwaltungsbehörden (1. Instanz) &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Landesregierungen (2. Instanz)&lt;/li&gt;&lt;li&gt;der Bund:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bezirksverwaltungsbehörden (1. Instanz)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Landeshauptmann (2. Instanz)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bundesminister (3. Instanz) &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Organ&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Abstrakt, dem Organ sind &lt;strong&gt;Organzuständigkeiten &lt;/strong&gt;zugeordnet, diese sind teil der Zuständigkeit der &lt;strong&gt;Organisation&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Verwaltungshandeln: &lt;/span&gt;Privatrechtliches Handeln &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gebietskörperschaften können als juristische Personen auch privatrechtlich handeln -&amp;gt; Fiskalverwaltung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Verwaltungshandeln: &lt;/span&gt;Schlicht-hoheitliches Handeln&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Hoheitliches Handeln, dass nicht auf dem Erlass von Rechtsnormen beruht.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Polizeistreife&lt;/li&gt;&lt;li&gt;Verkehrskontrolle&lt;/li&gt;&lt;li&gt;Urkundenausstellung&lt;/li&gt;&lt;li&gt;Auskunft durch Behörde&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Verwaltungshandeln: &lt;/span&gt;Maßnahme&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ausübung unmittelbarer verwaltungsbehördlicher Befehls- und Zwangsgewalt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;individueller Akt direkt auf gesetzlicher Grundlage z.B.: Festnahme&lt;/li&gt;&lt;li&gt;Wird wie Rechtsnorm mit Zwang durchgesetzt.&lt;/li&gt;&lt;li&gt;Anfechtung ungerechter Behandlung nicht möglich (anders als bei individueller Rechtsnorm = Bescheid) → Rechtsschutzlücke → Maßnahmebeschwerde vor Verwaltungsgericht (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel130" rel="noopener noreferrer" target="_blank"&gt;Art. 130 Abs. 1 Z. 1 B-VG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel132" rel="noopener noreferrer" target="_blank"&gt;Art. 132 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Verwaltungsverordnung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Wirkt nach innen, regelt die interne Verwaltungsorganisation&lt;/li&gt;&lt;li&gt;muss nicht kundgemacht werden (Abgrenzung zur Weisung schweirig)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Rechtsverordnung&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Wirkt nach außen&lt;/li&gt;&lt;li&gt;Legt Rechte und Pflichten für Bürger fest&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Ortspolizeiliche Verordnung&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Von Gemeinden erlassen &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(Art. 118 Abs. 6)&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;im eigenen Wirkungsbereich&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;nur zur Abwehr drohender oder bestehender Missstände&lt;/li&gt;&lt;li class="ql-indent-1"&gt;dürfen nicht gegen Bundes- oder Landesrecht verstoßen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Selbständige Verordnung&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;Ergehen unmittelbar aus Bundesverfassung (ohne weitere Gesetze)&lt;/li&gt;&lt;li&gt;Gesetzesergänzend, gesetzesvertretend oder gesetzesändernd.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Rechtsverordnung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Wirkt nach außen&lt;/li&gt;&lt;li&gt;Legt Rechte und Pflichten für Bürger fest&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Ortspolizeiliche Verordnung&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Von Gemeinden erlassen &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(Art. 118 Abs. 6)&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;im eigenen Wirkungsbereich&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;nur zur Abwehr drohender oder bestehender Missstände&lt;/li&gt;&lt;li class="ql-indent-1"&gt;dürfen nicht gegen Bundes- oder Landesrecht verstoßen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Arten von Verordnungen&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Durchführungsverordnung &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Selbständige Verordnung&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Ortspolizeiliche Verordnung&lt;/li&gt;&lt;li&gt;Rechtsverordnung&lt;/li&gt;&lt;li&gt;Verwaltungsverordnung&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Landesverwaltung: Landesregierung (Zuständigkeit, Zusammensetzung, Entscheidungsfindung, Wahl, Regierungsart, Amt)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Oberstes Organ der Landesverwaltung, zuständig für hoheitliche (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel11" rel="noopener noreferrer" target="_blank"&gt;Art. 11-15 B-VG&lt;/a&gt;) und nicht hoheitliche (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel17" rel="noopener noreferrer" target="_blank"&gt;Art. 17 B-VG&lt;/a&gt;) Verwaltung&lt;/li&gt;&lt;li&gt;Besteht aus Landeshauptmann und weiteren Landesräten (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel101" rel="noopener noreferrer" target="_blank"&gt;Art. 101 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Entscheidet als Kollegialorgan, Landesräte können teilweise auch als Einzelorgane tätig werden (Ämter der Landesregierungen)&lt;/li&gt;&lt;li&gt;Parlamentarisches System: Landtag wählt Regierung &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel101" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(136, 125, 220);"&gt;Art. 101 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Meist Mehrheitsregierung, außer in OÖ, NÖ und W → Proporzregierung=Konzentrationsregierung&lt;/li&gt;&lt;li&gt;Amt der Landesregierung: Hilfsapparat der Regierung &lt;strong&gt;&lt;em&gt;und &lt;/em&gt;&lt;/strong&gt;des Landeshauptmanns.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Grundrechtsquellen: Grundrechte im B-VG&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Gleichheitssatz (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel7" rel="noopener noreferrer" target="_blank"&gt;Art. 7 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Recht auf den gesetzlichen Richter (&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel83" rel="noopener noreferrer" target="_blank" style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Art. 83 Abs. 2 B-VG&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Recht der Richter auf Unabhängigkeit (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel87" rel="noopener noreferrer" target="_blank"&gt;Art. 87 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Recht der Gemeinden auf Selbstverwaltung (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank"&gt;Art. 116 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Weisungsfreie Vollziehung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Unabhängige &lt;strong&gt;Richter &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel87" rel="noopener noreferrer" target="_blank"&gt;Art. 87 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;weisungsfreier Teil der &lt;strong&gt;Justizverwaltung &lt;/strong&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel87" rel="noopener noreferrer" target="_blank"&gt;Art. 87 Abs. 2 B-VG&lt;/a&gt;): Richtersenate und Kommissionen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gemeindeselbstverwaltung&lt;/strong&gt;: Gemeinderat und Bürgermeister (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank" style="color: rgb(136, 125, 220); background-color: rgb(40, 45, 88);"&gt;Art. 116 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Weisungsfrei, unterliegen nur Aufsicht der Bundes/Landesbehörden.&lt;/li&gt;&lt;li&gt;Einfacher Bundes/Landesgesetzgeber kann weitere Verwaltungsorgane bei Rechtfertigung weisungsfrei stellen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel20" rel="noopener noreferrer" target="_blank"&gt;Art. 20 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie regelt die (Finanz)Verfassung wie der Staat zu seinem Geld kommt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Konstruiert den Staat als Abgabestaat&lt;/li&gt;&lt;li&gt;Staat bringt das Geld zwangsweise durch hoheitliche Abgaben, Gebühren und Beiträge auf.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie wird das Budget bestimmt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;In einem Budgetgesetz (Bundesfinanzgesetz) auf der Grundlage eines Bundesfinanzrahmengesetzes&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie nennt man das Geld- und Vermögensrelevante Handeln der Verwaltung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Gebarung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wo liegt die Budgethoheit, was bedeutet sie?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Beim Parlament, das Parlament entscheidet, wofür die Verwaltung welche Summen ausgeben darf. &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Sind Gemeinden unter dem Grundrechtsschutz?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ja, die Gemeindeautonomie (Recht auf Selbstverwaltung, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank"&gt;Art. 116 Abs. 1 B-VG&lt;/a&gt;)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wer ist ausgenommen aus dem Grundrechtsschutz?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Die Staaten (Bund und Land), die Grundrechte sind nicht dazu da den Staat vor sich selbst, Land vor dem Bund oder Bund vor dem Land zu schützen.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Können Gebietskörperschaften Träger von Grundrechten sein?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ja, juristische Personen&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (des öffentlichen und des Privatrechts)&lt;/span&gt; können Träger von Grundrechten sein, wenn dies &lt;strong&gt;wesensmäßig &lt;/strong&gt;möglich ist.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Gilt der Gleichheitssatz auch für die nicht-hoheitliche Verwaltung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ja, Diskriminierung ist verboten, und Sachlichkeit wird verlangt. &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Fiskalgeltung der Grundrechte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Die Bindung des Staates an die Grundrechte im Rahmen der Privatwirtschaftsverwaltung.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Die Verwaltung kann sowohl hoheitlich als auch privatrechtlich Handeln. Gilt der Grundrechtsschutz auch gegen die nicht-hoheitlichen Handlungen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ja&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie nennt man Verwaltungsakte des BP?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Entschließungen&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der Verwaltungsapparat des BP?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Präsidentschaftskanzl&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;ei&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine formalgesetzliche Delegation?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ein Gesetz bestimmt das Handeln der Vollziehung nicht oder nur sehr ungenau, dies ist verfassungswidrig (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel18" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(105, 122, 180);"&gt;Art 18. Abs 1. B-VG&lt;/a&gt;). Der Gesetzgeber delegiert daher die Pflicht das Recht zu bestimmen an die Vollziehung.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Verwaltungshandeln: Verordnung&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Verfassungsbegriff (Art. 139 B-VG)&lt;/li&gt;&lt;li&gt;Generelle (abstrakte oder konkrete) Anordnung einer Verwaltungsbehörde&lt;/li&gt;&lt;li&gt;Erst mit Kundmachung gültig&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Arten von Bescheiden&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Leistungsbescheid&lt;/strong&gt;: ordnet Tun oder Unterlassen an, &lt;strong&gt;vollstreckbar&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gestaltungsbescheid&lt;/strong&gt;: Gestaltet eine Rechtslage neu, &lt;strong&gt;nicht vollstreckbar&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Feststellungsbescheid&lt;/strong&gt;: verbindliche Feststellung einer unklaren Rechtslage, &lt;strong&gt;nicht vollstreckbar&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Formen des Verwaltungshandelns&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Bescheid&lt;/li&gt;&lt;li&gt;Verordnung&lt;/li&gt;&lt;li&gt;Maßnahme&lt;/li&gt;&lt;li&gt;Schlicht-hoheitliches Handeln&lt;/li&gt;&lt;li&gt;(Verwaltungsrechtlicher Vertrag)&lt;/li&gt;&lt;li&gt;Privatrechtliches Handeln&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Approbationsbefugnis&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Innerbehördliches Mandat&lt;/li&gt;&lt;li&gt;Organwalter kann Aufgaben an das Amt übertragen&lt;/li&gt;&lt;li&gt;Approbationsbefugte Beamte können damit "im Auftrag" der Behörde Bescheide oder Verordnungen erlassen, der Organwalter ist jedoch immer weisungsbefugt.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Amt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Einer Behörde zugeordneter bürokratischer Hilfsapparat, handelt nicht selbst hoheitlich. &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Behörde&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Verwaltungsorgane mit Rechtssetzungsbefugnissen (handeln hoheitlich)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Verwaltungsaufgabe&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Staatliche Aufgabe der Verwaltung einer Gebietskörperschaft&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Staatliche Aufgabe&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Öffentliche Aufgabe, die der Gesetzgeber dem Staat zuweist&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Aufgabe&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Organisation &lt;strong&gt;soll&lt;/strong&gt; in einer Sache handeln&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Pflichtaufgabe: muss Handeln&lt;/li&gt;&lt;li class="ql-indent-1"&gt;öffentliche Aufgabe: im Interesse der Allgemeinheit&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Zuständigkeit&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die &lt;strong&gt;Möglichkeit&lt;/strong&gt; einer Organisation in einer Sache zu handeln&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Organwalter (Definition, Zuordnung, Arten)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Den abstrakten Organen werden konkrete Menschen zugeordnet. &lt;/li&gt;&lt;li&gt;Gesetzessprache verwendet Organ und Organwalter oft synonym&lt;/li&gt;&lt;li&gt;Immer einer Gebietskörperschaft zugeordnet&lt;/li&gt;&lt;li&gt;Arten (Gesamtbegriff &lt;strong&gt;öffentliche Bedienstete&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Beamte = ernannte berufsmäßige Organe&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vertragsbedienstete = vertraglich bestellte Organe&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Organisation&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Abstrakte Konstrukte der Rechtsordnung denen bestimmte Aufgaben zukommen, bestehen meist aus vielen Organen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;z.B.: Gebietskörperschaft, Verwaltungsorganisation, Gerichtsorganisation&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Sicherheitsverwaltung: Was is das Bundesheer? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;militärische Formation des Bundes, zählt zur unmittelbaren Bundesverwaltung&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Sicherheitsbehörden des Bundes&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78a" rel="noopener noreferrer" target="_blank"&gt;Art. 78a-c B-VG&lt;/a&gt; richten die Sicherheitsbehörden ein&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/spg/paragraf/2" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;2 Abs. 2 SPG&lt;/a&gt; definiert Aufgaben der Sicherheitsverwaltung&lt;/li&gt;&lt;li&gt;2/3 Ebenen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;BM für Inneres&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Landespolizeidirektion&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bezirksverwaltungsbehörde&lt;/li&gt;&lt;li&gt;Mischform aus mittelbarer und unmittelbarer Bundesverwaltung, weil auf unterer Ebene teilweise Bezirksverwaltungsbehörden als Landesbehörden eingebunden sind&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Organwalter (Definition, Zuordnung, Arten)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Den abstrakten Organen werden konkrete Menschen zugeordnet. &lt;/li&gt;&lt;li&gt;Gesetzessprache verwendet Organ und Organwalter oft synonym&lt;/li&gt;&lt;li&gt;Immer einer Gebietskörperschaft zugeordnet&lt;/li&gt;&lt;li&gt;Arten (Gesamtbegriff &lt;strong&gt;öffentliche Bedienstete&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Beamte = ernannte berufsmäßige Organe&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vertragsbedienstete = vertraglich bestellte Organe&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;Durchführungsverordnung &lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Präzisiert ein Gesetz (&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel18" rel="noopener noreferrer" target="_blank" style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Art. 18 Abs. 2 B-VG&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;)&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Kompetenzverteilung in der nicht-hoheitlichen Verwaltung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel17" rel="noopener noreferrer" target="_blank"&gt;Art. 17 B-VG&lt;/a&gt;: Kompetenzverteilung in Art. 10 - 15 B-VG gilt &lt;strong&gt;nicht&lt;/strong&gt; für nicht-hoheitliche Verwaltung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das hoheitliche Organisationsrecht einer Gebietskörperschaft?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Bestimmt die innere Willensbildung des &lt;strong&gt;privatrechtlichen&lt;/strong&gt; Handelns&lt;/li&gt;&lt;li&gt;Zuständigkeit für Kaufverträge, Willensbildung, inhaltliche Gestaltung von Verträgen ⇾ bestimmt das hoheitliche Organisationsrecht (nicht die Privatrechtsordnung)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie funktioniert das Gesetzmäßigkeitsgebot in der nicht-hoheitlichen Verwaltung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Geregelt durch das Verwaltungsprivatrecht&lt;/li&gt;&lt;li&gt;&lt;strong&gt;differenziertes Legalitätsprinzip: &lt;/strong&gt;Auch privatrechtliche Handlungen unterliegen dem Gesetzmäßigkeitsgebot,  es ist aber flexibler und weniger streng, als für hoheitliches Handeln &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der Inhalt der nicht-hoheitlichen Verwaltung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Privatwirtschaftsverwaltung&lt;/li&gt;&lt;li&gt;Fiskalverwaltung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wer kann nicht-hoheitlich handeln, wer nicht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Nur die juristischen Personen: Bund, Länder und Gemeinden, also nur die Verwaltung. &lt;/li&gt;&lt;li&gt;Parlamente und Gerichte handeln  immer hoheitlich&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welche Gebietskörperschaften sind Träger von Privatrechten?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel17" rel="noopener noreferrer" target="_blank"&gt;Art. 17 B-VG&lt;/a&gt;: Bund und Länder sind juristische Personen&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank"&gt;Art. 116 Abs. 2 B-VG&lt;/a&gt;: Gemeinden sind juristische Personen&lt;/li&gt;&lt;li&gt;Vermögensfähig sind also der Bund, die Länder und die Gemeinden, nicht der Gesamtstaat Österreich.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Unterschiede zwischen juristischen Personen des Privatrechts und des öffentlichen Rechts? Was ist identisch? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Unterschiede:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Privatrecht: Durch Vertrag errichtet&lt;/li&gt;&lt;li class="ql-indent-1"&gt;öffentliches Recht: Durch Gesetz errichtet&lt;/li&gt;&lt;li&gt;Beide haben dieselbe (Privat)Rechtsfähigkeit, dieselben privaten Rechte und Pflichten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist ein Organisationsrecht? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Regelt welche Organe eine juristische Person hat, und welche Organwalter für die jur. Person handeln.&lt;/li&gt;&lt;li&gt;Insbesondere wer intern entscheidet, und wer nach außen vertritt.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Jur. Person handelt immer nur durch vertretungsbefugte Organe.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die zwei Kernaussagen der Wesenstheorie?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Umfang der Rechte von jur. Personen im wesentlichen auf &lt;strong&gt;Vermögensrechte &lt;/strong&gt;beschränkt = &lt;strong&gt;Vermögensfähigkeit&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Jur. Personen sind rechtsfähig, benötigen aber Menschen um für sie zu handeln (&lt;strong&gt;Organisationsrecht&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Können juristische Personen Rechtsträger sein? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Die Privatrechtsordnung erlaubt, dass juristische Personen von der Rechtsordnung als Rechtsträger behandelt wären, als wären sie Menschen.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind juristische Personen? &lt;/p&gt;&lt;p&gt;Wie werden sie noch genannt?&lt;/p&gt;&lt;p&gt;Wie wird entschieden, welche juristischen Personen es gibt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;= virtuelle Menschen&lt;/li&gt;&lt;li&gt;Auch Rechtsperson oder Körperschaft genannt&lt;/li&gt;&lt;li&gt;Gesetzgebung entscheidet ob und welche juristischen Personen es gibt.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind natürliche Personen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;= Menschen&lt;/li&gt;&lt;li&gt;Träger von Rechten und Pflichten&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;ABGB&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Allgemeines bürgerliches Gesetzbuch&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wer ist der gesetzliche Vertreter für ein Kind?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Die Eltern (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/167" rel="noopener noreferrer" target="_blank"&gt;§ 167 ABGB&lt;/a&gt;)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ist jeder Mensch handlungsfähig?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Nein (&lt;a href="https://www.jusline.at/gesetz/abgb/paragraf/21" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;21 ABGB&lt;/a&gt;), wer nicht handlungsfähig ist, braucht einen Vertreter der für ihn handelt&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Handlungsfähigkeit?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die Fähigkeit, durch eigenes Handeln Rechte zu erwerben und Pflichten zu begründen.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Rechtsfähigkeit? Wer hat sie wie lange? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die Fähigkeit, Träger privater Rechte und Pflichten zu sein (z.B.: Eigentümer von Geld und Vermögen)&lt;/li&gt;&lt;li&gt;Jeder Mensch ist von Geburt bis zum Tod rechtsfähig.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Einzelne Grundrechte&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Eigentumsfreiheit&lt;/li&gt;&lt;li&gt;Erwerbsfreiheit&lt;/li&gt;&lt;li&gt;Recht auf persönliche Freiheit&lt;/li&gt;&lt;li&gt;Hausrecht&lt;/li&gt;&lt;li&gt;Versammlungsfreiheit&lt;/li&gt;&lt;li&gt;Meinungsfreiheit&lt;/li&gt;&lt;li&gt;...&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Recht auf den gesetzlichen Richter?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(102, 102, 102);"&gt; Justizgrundrecht, das festlegt, dass für Rechtsstreitigkeiten und Prozesse bereits im Voraus bestimmt sein muss, welches&amp;nbsp;&lt;/span&gt;Gericht&amp;nbsp;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(102, 102, 102);"&gt;und welcher Richter zuständig ist (&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel83" rel="noopener noreferrer" target="_blank"&gt;Art.&amp;nbsp;83 Abs. 2&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel87" rel="noopener noreferrer" target="_blank"&gt;Art. 87 Abs. 3&amp;nbsp;B-VG&lt;/a&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(102, 102, 102);"&gt;)&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Verfahrensgrundrechte&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Wehren den Staat nicht ab, sondern verlangen Einhaltung der durch die Verfassung gewährleisteten Verfahrensrechte &lt;/li&gt;&lt;li&gt;Beispiele: Recht auf den gesetzlichen Richter, Recht auf faires Verfahren, keine Strafe ohne Gesetz.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Politische Grundrechte (= Teilhaberechte)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Durch die Verfassung gewährleistete Recht der Teilnahme der Menschen am Staat&lt;/li&gt;&lt;li&gt;Keine Abwehrrechte, sondern Teilhaberechte (status activus)&lt;/li&gt;&lt;li&gt;Aktive Teilhabe an der Staatswillensbildung und Staatsgewalt&lt;/li&gt;&lt;li&gt;Beispiele: Wahlrecht, Recht auf Volksbegehren, Petitionsrecht, Gründung und Betätigungsfreiheit polit. Parteien.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Soziale Grundrechte&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Österreich ist ein Sozialstaat, die Verfassung kennt aber &lt;strong&gt;keine&lt;/strong&gt; sozialen Grundrechte.&lt;/li&gt;&lt;li&gt;Begründung: könnten den Staat wirtschaftlich überfordern.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Freiheitsrechte mit staatlichen Schutzpflichten&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Nicht nur Abwehrrecht gegen Staat&lt;/li&gt;&lt;li&gt;Anspruch gegen den Staat, dass er den Freiraum auch vor Beschädigung durch andere Privatpersonen schützt&lt;/li&gt;&lt;li&gt;Beispiele: Recht auf Leben (Art. 2 EMRK), Verbot der Folter, ..&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Freiheitsrechte ohne Gesetzesvorbehalt&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Absolut schützendes Freiheitsrecht&lt;/li&gt;&lt;li&gt;Kein Eingriff in den Schutzbereich durch einfache Gesetze zulässig&lt;/li&gt;&lt;li&gt;Beispiele: Verbot der Folter, Verbot der Todesstrafe, ... &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wann ist die Zustimmung der Bundesregierung für ein Landesgesetz notwendig? Wie wird die Zustimmung eingeholt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;Bundesorgane sollen bei Vollziehung mitwirken (&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel97" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Art. 97 Abs. 2 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Ein eigenes Statut (Stadtrecht) ist betroffen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel116" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 116 Abs. 3 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;Änderung der Organisation der Behörden der allg. staatlichen Verwaltung in den Ländern (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel15" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 15 Abs. 10 B-VG)&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Der LH muss vor Kundmachung dem Bundeskanzleramt bekannt das Gesetz geben. Regierung hat 8 Wochen für Ablehnung&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Quoren für Landesverfassungsgesetze?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Präsenz 1/2, Konsens 2/3 (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel99" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 99 Abs. 2 B-VG&lt;/a&gt;)&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Zuständigkeit&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Die &lt;strong&gt;Möglichkeit&lt;/strong&gt; einer Organisation in einer Sache zu handeln&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Arten der Leitung der Verwaltung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Aufsicht: &lt;/strong&gt;ex post - nach der Handlung&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Rechtsaufsicht: gesetzmäßig&lt;/li&gt;&lt;li&gt;Zweckaufsicht: zweckmäßig&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;strong&gt;Weisung: &lt;/strong&gt;ex ante - vor der Handlung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Verwaltungshandeln: Bescheid&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Verfassungsbegriff (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel130" rel="noopener noreferrer" target="_blank"&gt;Art. 130 Abs. 1 B-VG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel132" rel="noopener noreferrer" target="_blank"&gt;Art. 132 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;3 formale Merkmale (nicht vorhanden: Absolut nichtig)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es muss eine Verwaltungsbehörde handeln&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es muss an einen individuellen Adressaten gerichtet sein&lt;/li&gt;&lt;li class="ql-indent-1"&gt;es muss eine behördliche Anordnung enthalten&lt;/li&gt;&lt;li&gt;Gesetzgeber kann weitere Merkmale hinzufügen, Auswirkung des Fehlens legt Gesetzgeber fest (z.B.: relativ nichtig)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Aufgabe&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Organisation &lt;strong&gt;soll&lt;/strong&gt; in einer Sache handeln&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Pflichtaufgabe: muss Handeln&lt;/li&gt;&lt;li class="ql-indent-1"&gt;öffentliche Aufgabe: im Interesse der Allgemeinheit&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Staatliche Aufgabe&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Öffentliche Aufgabe, die der Gesetzgeber dem Staat zuweist&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Verwaltungsaufgabe&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Staatliche Aufgabe der Verwaltung einer Gebietskörperschaft&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Behörde&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Verwaltungsorgane mit Rechtssetzungsbefugnissen (handeln hoheitlich)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Amt&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Einer Behörde zugeordneter bürokratischer Hilfsapparat, handelt nicht selbst hoheitlich. &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Approbationsbefugnis&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Innerbehördliches Mandat&lt;/li&gt;&lt;li&gt;Organwalter kann Aufgaben an das Amt übertragen&lt;/li&gt;&lt;li&gt;Approbationsbefugte Beamte können damit "im Auftrag" der Behörde Bescheide oder Verordnungen erlassen, der Organwalter ist jedoch immer weisungsbefugt.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Formen des Verwaltungshandelns&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Bescheid&lt;/li&gt;&lt;li&gt;Verordnung&lt;/li&gt;&lt;li&gt;Maßnahme&lt;/li&gt;&lt;li&gt;Schlicht-hoheitliches Handeln&lt;/li&gt;&lt;li&gt;(Verwaltungsrechtlicher Vertrag)&lt;/li&gt;&lt;li&gt;Privatrechtliches Handeln&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Eingriffsvorbehalt vs. Ausgestaltungsvorbehalt bei Freiheitsrechten&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Eingriffsvorbehalt &lt;/strong&gt;erlaubt in den Schutzbereich des Freiheitsrechts einzugreifen, und diesen durch Gesetz einzuschränken&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ausgestaltungsvorbehalt &lt;/strong&gt;erlaubt  nur ein Freiheitsrecht näher auszugestalten, nicht in den Schutzbereich einzugreifen.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was besagt die Wesensgehaltssperre?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ein Freiheitsrecht darf durch einen gesetzlichen Eingriff nicht hinfällig werden, ein Minimum an Freiheit muss bestehen bleiben.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Wie muss der Gesetzgeber handeln, wenn der Verfassungstext keine Vorgaben für einen gesetzlichen Eingriff auf ein Freiheitsrecht hat? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Es wird die Auslegung herangezogen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Gesetzgeber muss nachweislich ein konkretes öffentliches Interesse verfolgen&lt;/li&gt;&lt;li&gt;Der Eingriff muss verhältnismäßig sein (Verhältnismäßigkeitsgrundsatz), die Belastung der Freiheit darf nicht höher sein, als zur Erreichung des öffentlichen Interesses unbedingt erforderlich&lt;/li&gt;&lt;li&gt;Eingriff muss sachlich sein&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Freiheitsrechte mit Gesetzesvorbehalt&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Relativ schützendes&lt;/strong&gt; Freiheitsrecht&lt;/li&gt;&lt;li&gt;Eingriff in den Schutzbereich durch einfache Gesetze möglich - unter Beachtung der &lt;strong&gt;materiellen Eingriffsschranken&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Steht unter materiellem Gesetzesvorbehalt, weil der Gesetzgeber bei seinen Regelungen inhaltlich an Vorhaben der Verfassung gebunden ist.&lt;/li&gt;&lt;li&gt;Der Verfassungstext sagt, ob ein Grundrecht unter materiellem Gesetzesvorbehalt steht&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Beispiele für Freiheitsrechte&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Eigentumsfreiheit&lt;/li&gt;&lt;li&gt;Erwerbsfreiheit&lt;/li&gt;&lt;li&gt;Kunstfreiheit&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Freiheitsrechte, warum heißen sie auch Abwehrrechte?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Grundrechte, durch welche die Verfassung den Menschen Freiräume gewährleistet.&lt;/li&gt;&lt;li&gt;Erlauben dem einzelnen verfassungswidrige Eingriffe des Staats in den geschützten Freiraum abzuwehren (über den dafür vorgesehenen besonderen Prozessweg) &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Schützt der Gleichheitssatz vor eingriffen in den Freiraum der Menschen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Nein, er ist kein Freiheitsrecht&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Willkürverbot, was ist Willkür?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Gilt für die Vollziehung&lt;/li&gt;&lt;li&gt;Verbot willkürlicher Entscheidungen&lt;/li&gt;&lt;li&gt; Willkür liegt vor, wenn eine Behörde&lt;/li&gt;&lt;li class="ql-indent-1"&gt;eine Person absichtlich benachteiligt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ohne Rechtsgrundlage entscheidet&lt;/li&gt;&lt;li class="ql-indent-1"&gt;die Rechtslage verkennt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gravierende Verfahrensfehler begeht&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wen bindet der Gleichheitssatz, wen nicht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Bindet den:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;einfachen Bundesgesetzgeber&lt;/li&gt;&lt;li&gt;einfachen Landesgesetzgeber&lt;/li&gt;&lt;li&gt;Landesverfassungsgesetzgeber&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Bindet nicht:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bundesverfassungsgesetzgeber, weil der Gleichheitssatz bloß ein Bundesverfassungsgesetz ist. &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wann verletzt ein einfaches Gesetz den Gleichheitssatz?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wenn es:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Unsachliche Differenzierungen vornimmt&lt;/strong&gt; (Gleiches ist gleich zu behandeln, soweit kein Grund für eine Ungleichbehandlung vorliegt)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gebotene Differenzierungen unterlässt&lt;/strong&gt; (Ungleiches darf nicht ohne Grund gleich behandelt werden)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Sachlich nicht gerechtfertigte Regelungen&lt;/strong&gt; trifft.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Gleichheitsformel&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Eine Ungleichbehandlung ist &lt;strong&gt;gleichheitskonform&lt;/strong&gt;, wenn sie sachlich gerechtfertigt ist. Eine Ungleichbehandlung ist &lt;strong&gt;gleichheitswidrig&lt;/strong&gt;, wenn sie &lt;strong&gt;nicht &lt;/strong&gt;sachlich gerechtfertigt ist.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;(z.B.: Matura als Voraussetzung für Studium ist konform, da allgemeine Vorbildung notwendig ist, um sinnvoll zu studieren)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Kann der Gesetzgeber ungleiches gleich behandeln?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Nein, bei unterschieden im Tatsächlichen (z.B.: unterschiedliches Einkommen) muss der Gesetzgeber auch unterschiedliche Regelungen erlassen (Gebot &lt;strong&gt;sachlicher Differenzierung&lt;/strong&gt;) &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was bedeutet &lt;strong&gt;gleich&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Gleiche Betroffenheit der Rechtsunterworfenen unter Berücksichtigung aller rechtlichen und tatsächlichen Wirkungen&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Gleichheitsrechte&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Gleichheitssatz: &lt;a href="https://www.jusline.at/gesetz/stgg/paragraf/artikel2" rel="noopener noreferrer" target="_blank"&gt;Art 2. StGG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel7" rel="noopener noreferrer" target="_blank"&gt;Art 7 Abs. 1 B-VG&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Recht auf Gleichbehandlung von Fremden untereinander&lt;/li&gt;&lt;li class="ql-indent-1"&gt;BVG über die Beseitigung aller Formen rassischer Diskriminierung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welche Kategorien/Arten von Grundrechten gibt es?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Gleichheitsrechte (Gleichheitssatz)&lt;/li&gt;&lt;li&gt;Freiheitsrechte (= Abwehrrechte)&lt;/li&gt;&lt;li&gt;Soziale Grundrechte&lt;/li&gt;&lt;li&gt;Politische Grundrechte (= Teilhaberechte)&lt;/li&gt;&lt;li&gt;Verfahrensgrundrechte&lt;/li&gt;&lt;li&gt;Sonstige Grundrechte&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind verfassungsimmanente&amp;nbsp;Schranken? Was bedeuten Sie für Grundrechte? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Einschränkung des Schutzbereichs des Grundrechts durch andere Grundrechte und objektive Verfassungsbestimmungen.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Der Schutzbereich des Grundrechts geht daher nicht zwangsläufig so weit, wie die Formulierung des Textes erwarten lässt.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie wird mit Widersprüchen in Grundrechtsquellen umgegangen? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Dasselbe Grundrecht kann an verschiedenen Stellen der Verfassungsordnung verankert sein. Widersprüche sind nach den Regeln der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;Derogation &lt;/strong&gt;aufzulösen.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie unterteilt die Verfassung unter objektivem Recht gewährleistete Rechte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Nach Adressatenkreis in Staatsbürgerrechte und Menschenrechte&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Drittwirkung der Grundrechte&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Durch Trennung von Staat und Gesellschaft gibt es &lt;strong&gt;keine Drittwirkung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Grundrechte gelten nur gegen den Staat, nicht Mensch gegen Mensch&lt;/li&gt;&lt;li&gt;Ausnahmen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gesetzlich angeordnete Drittwirkungen (z.B.: Datenschutzgesetz)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Grundrechte mit staatlicher Schutzpflicht (Recht auf Leben)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Mittelbare Drittwirkung im Zivilrecht (Auslegung, Sittenklauseln)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wo werden über Verstöße gegen Grundrechte entschieden?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;OGH&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wo werden in der Regel über Verstöße gegen subjektives Recht entschieden?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;im VfGH&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie wird der Schutzbereich eines Grundrechts festgelegt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Die Verfassung die ein Grundrecht normiert, legt den Schutzbereich mit dem Wortlaut des Verfassungstextes fest. Diese Begriffe sind allerdings auslegungsbedürftig (z.&amp;nbsp;B.: Eigentumsfreiheit hat den Schutzbereich "Eigentum")&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Grundrechtsquellen: Einzelne Grundrechte in Staatsverträgen&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Rechte der Minderheiten&lt;/li&gt;&lt;li&gt;Religionsfreiheit&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Grundrechtsquellen: Grundrechte in einfachen Gesetzen&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Recht auf Zivildienst&lt;/li&gt;&lt;li&gt;Recht auf Datenschutz&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Grundrechtsquellen&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Quellen:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Grundrechtskataloge&lt;/li&gt;&lt;li&gt;Grundrechtsgesetze&lt;/li&gt;&lt;li&gt;Grundrechte im B-VG&lt;/li&gt;&lt;li&gt;Grundrechte in einfachen Gesetzen&lt;/li&gt;&lt;li&gt;Einzelne Grundrechte in Staatsverträgen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Grundrechtsquellen: Grundrechtsgesetze&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Hausrechts Gesetz &lt;/li&gt;&lt;li&gt;Beschluss der provisorischen Nationalversammlung über die Aufhebung der Zensur 1918&lt;/li&gt;&lt;li&gt;PersFrG (Bundesverfassungsgesetz zum Schutz der persönlichen Freiheit)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Grundrechtsquellen: Grundrechtskataloge&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;StGG 1867&lt;/li&gt;&lt;li&gt;EMRK + ZP&lt;/li&gt;&lt;li&gt;BVG Kinderrechte&lt;/li&gt;&lt;li&gt;EU Grundrechtecharta&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Gegen wen schützen Grundrechte, gegen wen nicht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Grundrechte schützen gegen Staat und Staatsgewalt&lt;/li&gt;&lt;li&gt;Schützen auch gegen den Gesetzgeber&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gegen einfachen Bundesgesetzgeber&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gegen Landesverfassungsgesetzgeber&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gegen einfachen Landesgesetzgeber&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gegen die staatl. Vollziehung (Verwaltung und Gerichtsbarkeit)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aber: &lt;/strong&gt;Bundesverfassungsgesetze können Grundrechte einschränken. (z.&amp;nbsp;B.: Wehrpflicht für Männer widerspricht dem Gleichheitssatz, ist aber durch B-VG diskriminierend festgelegt) &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Objektives Recht&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Mensch hat keinen durchsetzbaren Anspruch auf Einhaltung der Gesetze&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Subjektives Recht&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Grundrechte sind gegen den Staat durchsetzbare Individualrechte&lt;/li&gt;&lt;li&gt;Mensch hat Anspruch auf Einhaltung der Gesetze (Verwaltung, Gerichtsbarkeit, Gesetzgebung verfolgen Verletzung der Grundrechte)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Grundrechte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Alle den Menschen durch formelle Verfassungsgesetze gewährleistete Recht&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Geschichte der Grund- und Freiheitsrechte&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;1789&lt;/strong&gt;: Deklaration der Menschen- und Bürgerrechte&lt;/p&gt;&lt;p&gt;&lt;strong&gt;1867&lt;/strong&gt;: Staatsgrundgesetz (Dezemberverfassung) &lt;/p&gt;&lt;p&gt;&lt;strong&gt;1948&lt;/strong&gt;: Allgemeine Erklärung der Menschenrechte&lt;/p&gt;&lt;p&gt;&lt;strong&gt;1950&lt;/strong&gt;: Europäische Menschenrechtskonvention&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Arten von Bescheiden&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Leistungsbescheid&lt;/strong&gt;: ordnet Tun oder Unterlassen an, &lt;strong&gt;vollstreckbar&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gestaltungsbescheid&lt;/strong&gt;: Gestaltet eine Rechtslage neu, &lt;strong&gt;nicht vollstreckbar&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Feststellungsbescheid&lt;/strong&gt;: verbindliche Feststellung einer unklaren Rechtslage, &lt;strong&gt;nicht vollstreckbar&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Verwaltungshandeln: Verordnung&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Verfassungsbegriff (Art. 139 B-VG)&lt;/li&gt;&lt;li&gt;Generelle (abstrakte oder konkrete) Anordnung einer Verwaltungsbehörde&lt;/li&gt;&lt;li&gt;Erst mit Kundmachung gültig&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(34, 38, 74); color: rgb(238, 236, 246);"&gt;Wachkörper: &lt;/span&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Gemeindewachkörper &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel118" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 118 Abs. 8 B-VG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel118a" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 118a B-VG&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(226, 148, 20);"&gt;Gemeinde&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Aufgaben im kommunalen Bereich&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(34, 38, 74); color: rgb(238, 236, 246);"&gt;Wachkörper: &lt;/span&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Justizwache &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/stvg/paragraf/13a" rel="noopener noreferrer" target="_blank" style="color: rgb(105, 122, 180); background-color: rgb(40, 45, 88);"&gt;§&amp;nbsp;13a Strafvollzugsgesetz&lt;/a&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;﻿Bund&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Bewachung der Strafgefangenen&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(34, 38, 74); color: rgb(238, 236, 246);"&gt;Wachkörper: &lt;/span&gt;Bundespolizei&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel10" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(105, 122, 180);"&gt;Art. 10 Abs. 1 Z. 14 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;, &lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78d" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(105, 122, 180);"&gt;Art 78d B-VG&lt;/a&gt;&lt;/li&gt;&lt;li&gt;Bund&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Innere Sicherheit&lt;/span&gt;&lt;/li&gt;&lt;li&gt;Unmittelbare Bundesverwaltung, BM für Inneres an der Spitze&lt;/li&gt;&lt;li&gt;im Bereich jeder Landespolizeidirektion sind Bezirkskommanden bzw. Stadtpolizeikommanden eingerichtet&lt;/li&gt;&lt;li&gt;Wachkörper Bundespolizei ist von Sicherheitsbehörden des Bundes zu unterscheiden!&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wachkörper&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Bewaffnete Formationen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78d" rel="noopener noreferrer" target="_blank"&gt;Art. 78d Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bundespolizei: &lt;strong&gt;Bund&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Justizwache: &lt;strong&gt;Bund&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gemeindewachkörper: &lt;strong&gt;Gemeinde&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Organisation und Führung der Bundespolizei und die Org. sonstiger Wachkörper (Ausnahme: Gemeindewachkörper) ist Bundessache&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Sicherheitsbehörden: &lt;/span&gt;Bezirksverwaltungsbehörde&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Bezirkshauptmannschaft/Bürgermeister besorgt prinzipiell Sicherheitsverwaltung auf Bundesebene&lt;/li&gt;&lt;li&gt;Als Verwaltungsbehörde aber nicht auf Sicherheitsaufgaben spezialisiert.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Sicherheitsbehörden: Landespolizeidirektion&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78b" rel="noopener noreferrer" target="_blank" style="color: rgb(105, 122, 180); background-color: rgba(0, 0, 0, 0);"&gt;Art. 78b Abs. 1 B-VG&lt;/a&gt;) für jedes Bundesland:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Landespolizeidirektor weisungsgebunden an BM&lt;/li&gt;&lt;li class="ql-indent-1"&gt;BM muss jede wichtige Weisung an den LH mitteilen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;BM kann Landespolizeidirektor nur mit Einvernehmen des LH bestellen&lt;/li&gt;&lt;li&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78c" rel="noopener noreferrer" target="_blank"&gt;Art. 78c B-VG&lt;/a&gt; ermächtigt einfachen Bundesgesetzgeber die Landespolizeidirektion zur Sicherheitsbehörde 1. Instanz zu bestimmen, &lt;a href="https://www.jusline.at/gesetz/spg/paragraf/8" rel="noopener noreferrer" target="_blank"&gt;§&amp;nbsp;8 SPG&lt;/a&gt; legt dafür einige Gebiete fest.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Sicherheitsbehörden: BM für Inneres&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78a" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 78a Abs. 1 B-VG&lt;/a&gt;): Generaldirektion für öffentliche Sicherheit sorgt für Sicherheitsverwaltung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;SPG&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Sicherheitspolizeigesetz&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Abgabebehörden&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Auftragsverwaltung des Bundes: für nicht-hoheitliche Verwaltung ist theoretisch nur der BM zuständig (z.&amp;nbsp;B.: Bundesvermögen, Geschäfte des Bundes)&lt;/li&gt;&lt;li&gt;BM kann einzelne Geschäfte durch hoheitlichen Auftrag dem LH übertragen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel104" rel="noopener noreferrer" target="_blank"&gt;Art. 104 Abs. 2&lt;/a&gt;) &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Unmittelbare Bundesverwaltung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel102" rel="noopener noreferrer" target="_blank" style="background-color: rgb(40, 45, 88); color: rgb(105, 122, 180);"&gt;Art. 102 Abs. 2 B-VG&lt;/a&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ausnahme&lt;/li&gt;&lt;li&gt;Bund erledigt Aufgaben durch eigene Bundesbehörden&lt;/li&gt;&lt;li&gt;Bund darf dennoch mittelbare Bundesverwaltung nutzen &lt;/li&gt;&lt;li&gt;Mit Zustimmung der Länder, darf Bund auch Materien regeln, die nicht in Art. 102 Abs. 2 stehen (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel102" rel="noopener noreferrer" target="_blank"&gt;Art. 102 Abs. 4 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Mittelbare Bundesverwaltung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;(&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel102" rel="noopener noreferrer" target="_blank"&gt;Art. 102 Abs. 1 B-VG&lt;/a&gt;)&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Das oberste Organ ist ein BM (oder der BK), als funktionelles und organisatorisches Organ des Bundes&lt;/li&gt;&lt;li&gt;Das mittlere Organ ist der Landeshauptmann (als Einzelorgan). &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Organisatorisch ein Landesorgan, funktionell aber im Auftrag des Bundes&lt;/li&gt;&lt;li class="ql-indent-1"&gt;An Weisungen des BM gebunden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Amt: Amt der Landesregierung&lt;/li&gt;&lt;li&gt;Das untere Organ ist die Bezirksverwaltungsbehörde&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Organwalter (Bezirkshauptmann/Bürgermeister) an Weisung des LH gebunden (In Bundesverwaltung, sonst an Landesregierung)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Amt: Bezirkshauptmannschaft/Magistrat&lt;/li&gt;&lt;li&gt;Unterste Organe: Gemeindeorgane&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Staatssekretäre &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Werden zwar in Art. 19 B-VG als oberste Organe der Verwaltung genannt, sind jedoch BM unterstellt und weisungsgebunden (&lt;/span&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78" rel="noopener noreferrer" target="_blank" style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Art. 78 Abs. 3 B-VG&lt;/a&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Aufgabe ist Unterstützung und Vertretung des BM, sie sind nicht Teil der Bundesregierung&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ämter der Bundesregierung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Bundeskanzleramt für BK&lt;/li&gt;&lt;li&gt;Bundesministerien für die BM&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Bundesregierung: &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;BK, VK und BMs als Einzelorgane&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Oberste Organe der Verwaltung (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel19" rel="noopener noreferrer" target="_blank"&gt;Art. 19 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li&gt;BM für Finanzen und für Inneres sind in der Verfassung, andere werden durch Bundesministeriengesetz 1986 bestimmt&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Bundesregierung &lt;/span&gt;als Kollegialorgan&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;= Ministerrat&lt;/li&gt;&lt;li&gt;Beschlüsse müssen einstimmig sein&lt;/li&gt;&lt;li&gt;Aufgabe sind Regierungsakte wie&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vorschläge an BP (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel67" rel="noopener noreferrer" target="_blank"&gt;Art. 67 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesetzesvorlagen an das Parlament (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel41" rel="noopener noreferrer" target="_blank"&gt;Art. 41 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vorschläge für Ernennung von Verfassungsrichtern (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel147" rel="noopener noreferrer" target="_blank"&gt;Art. 147 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Zusammensetzung der Bundesregierung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Besteht aus BK, Vizekanzler und Bundesministern (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel19" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt;Art. 19 Abs. 1 B-VG&lt;/a&gt;,&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel69" rel="noopener noreferrer" target="_blank" style="background-color: rgba(0, 0, 0, 0); color: rgb(105, 122, 180);"&gt; Art. 69 Abs. 1 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Landesverwaltung unterhalb der Regierung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Landesverwaltung in Verwaltungssprengel territorial gegliedert&lt;/li&gt;&lt;li&gt;Land in Bezirke gegliedert, 2 Arten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bezirk&lt;/strong&gt;, der mehrere Gemeinden erfasst&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Statutarstadt&lt;/strong&gt;, die alleine ein Bezirk ist&lt;/li&gt;&lt;li&gt;Bezirksverwaltungsbehörden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bezirkshauptmann (monokratisch), Amt: Bezirkshauptmannschaft&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bürgermeister, Amt: Magistrat&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Sicherheitsverwaltung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Sicherheitsbehörden des Bundes (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel78a" rel="noopener noreferrer" target="_blank"&gt;Art. 78a-c B-VG&lt;/a&gt;)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ortspolizei&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Örtliche Verwaltungspolizei und örtliche Sicherheitspolizei gemeinsam&lt;/li&gt;&lt;li&gt;bei gesetzlicher Lücke zur Beseitigung konkreter Gefahren und Missstände, wenn diese das "örtliche Gemeinschaftsleben" stören &lt;/li&gt;&lt;li&gt;Gemeinde darf gesetzesergänzende Verordnungen erlassen (ortspolizeiliche Verordnungen &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel118" rel="noopener noreferrer" target="_blank"&gt;Art. 118 Abs. 6 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Örtliche Sicherheitspolizei&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Aus dem Kompetenztatbestand ausgenommen → Aufteilung in überörtliche und örtliche Sicherheitspolizei&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Sicherheitspolizei&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel10" rel="noopener noreferrer" target="_blank" style="color: rgb(105, 122, 180); background-color: rgb(40, 45, 88);"&gt;Art. 10 Abs. 1 Z. 7 B-VG&lt;/a&gt; Aufrechterhaltung der öffentlichen Ruhe, Ordnung und Sicherheit (soweit keiner konkreten Sachmaterie zugewiesen)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Örtliche Verwaltungspolizei&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Alle in &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel10" rel="noopener noreferrer" target="_blank" style="color: rgb(105, 122, 180); background-color: rgb(40, 45, 88);"&gt;Art. 10-15 B-VG&lt;/a&gt; enthaltenen Angelegenheiten der Verwaltungspolizei, die im &lt;em&gt;örtlichen Interesse&lt;/em&gt; gelegen sind, fallen in den Wirkungsbereich der Gemeinden&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Verwaltungspolizei&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Staatliches Handeln zur Abwehr und Beseitigung konkreter Gefahren und Missstände&lt;/li&gt;&lt;li&gt;Annexmaterie zu den Kompetenzen in &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel10" rel="noopener noreferrer" target="_blank"&gt;Art. 10-15 B-VG&lt;/a&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Allgemeine staatliche Verwaltung (Aufstellung in Bund und Ländern)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Allzuständigkeit der Staatsgewalt, erledigt von allgemeinen staatlichen Verwaltungsorganen&lt;/li&gt;&lt;li&gt;der Länder: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bezirksverwaltungsbehörden (1. Instanz) &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Landesregierungen (2. Instanz)&lt;/li&gt;&lt;li&gt;der Bund:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bezirksverwaltungsbehörden (1. Instanz)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Landeshauptmann (2. Instanz)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bundesminister (3. Instanz) &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Organ&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Abstrakt, dem Organ sind &lt;strong&gt;Organzuständigkeiten &lt;/strong&gt;zugeordnet, diese sind teil der Zuständigkeit der &lt;strong&gt;Organisation&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Verwaltungshandeln: &lt;/span&gt;Privatrechtliches Handeln &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Gebietskörperschaften können als juristische Personen auch privatrechtlich handeln -&amp;gt; Fiskalverwaltung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Verwaltungshandeln: &lt;/span&gt;Schlicht-hoheitliches Handeln&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Hoheitliches Handeln, dass nicht auf dem Erlass von Rechtsnormen beruht.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Polizeistreife&lt;/li&gt;&lt;li&gt;Verkehrskontrolle&lt;/li&gt;&lt;li&gt;Urkundenausstellung&lt;/li&gt;&lt;li&gt;Auskunft durch Behörde&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Verwaltungshandeln: &lt;/span&gt;Maßnahme&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Ausübung unmittelbarer verwaltungsbehördlicher Befehls- und Zwangsgewalt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;individueller Akt direkt auf gesetzlicher Grundlage z.B.: Festnahme&lt;/li&gt;&lt;li&gt;Wird wie Rechtsnorm mit Zwang durchgesetzt.&lt;/li&gt;&lt;li&gt;Anfechtung ungerechter Behandlung nicht möglich (anders als bei individueller Rechtsnorm = Bescheid) → Rechtsschutzlücke → Maßnahmebeschwerde vor Verwaltungsgericht (&lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel130" rel="noopener noreferrer" target="_blank"&gt;Art. 130 Abs. 1 Z. 1 B-VG&lt;/a&gt;, &lt;a href="https://www.jusline.at/gesetz/b-vg/paragraf/artikel132" rel="noopener noreferrer" target="_blank"&gt;Art. 132 Abs. 2 B-VG&lt;/a&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Verwaltungsverordnung&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Wirkt nach innen, regelt die interne Verwaltungsorganisation&lt;/li&gt;&lt;li&gt;muss nicht kundgemacht werden (Abgrenzung zur Weisung schweirig)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;3 Rechtsordnungen&lt;/p&gt;</t>
@@ -1900,7 +2002,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B250"/>
+  <dimension ref="A1:B267"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -3906,6 +4008,142 @@
         <v>499</v>
       </c>
     </row>
+    <row r="251" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A264" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>